<commit_message>
Another version - consider final
</commit_message>
<xml_diff>
--- a/sample_timeline.xlsx
+++ b/sample_timeline.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Time Elapsed (in months for 3 yr study)</t>
   </si>
@@ -66,7 +66,7 @@
     <t>Literature Review</t>
   </si>
   <si>
-    <t>Characterizing a Visual SLAM System With Ego-motion, Camera Viewpoint and Environmental Conditions</t>
+    <t>Visual Odometry and Place Recognition Robustness to Variations in Environment and Ego-motion</t>
   </si>
   <si>
     <t>Semantics for Visual Place Recognition</t>
@@ -90,13 +90,10 @@
     <t>Performance Evaluation of Visual SLAM Using High Fidelity Simulation</t>
   </si>
   <si>
-    <t>Adapting Place Recognition to Variations Within Environment</t>
-  </si>
-  <si>
     <t>Hybrid Visual Odometry for Low Light and Rapid Movement</t>
   </si>
   <si>
-    <t>Robust Semantic Representation</t>
+    <t>Improving Visual Place Recognition From Motion Cues</t>
   </si>
   <si>
     <r>
@@ -132,6 +129,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Within</t>
     </r>
@@ -140,15 +138,13 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Places</t>
     </r>
   </si>
   <si>
-    <t>Condition-Invariant 3D Relative Pose Estimation for Loop Closures</t>
-  </si>
-  <si>
-    <t>SLAM for Semantics</t>
+    <t>Appearance-Robust 3-D Relative Pose Estimation</t>
   </si>
   <si>
     <t>An Integrated System</t>
@@ -219,7 +215,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -276,17 +272,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -400,7 +385,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -494,10 +479,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -612,10 +593,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="1:40"/>
+  <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -16196,7 +16177,7 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="22"/>
@@ -17223,7 +17204,7 @@
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="21" t="s">
         <v>25</v>
       </c>
@@ -18251,7 +18232,7 @@
       <c r="AMI24" s="0"/>
       <c r="AMJ24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="21" t="s">
         <v>26</v>
       </c>
@@ -18259,10 +18240,10 @@
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
+      <c r="F25" s="22"/>
       <c r="G25" s="23"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="0"/>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
@@ -19280,7 +19261,7 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="22"/>
@@ -19288,10 +19269,10 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
-      <c r="J26" s="22"/>
+      <c r="J26" s="23"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
@@ -20308,7 +20289,7 @@
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="22"/>
@@ -20318,9 +20299,9 @@
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
+      <c r="I27" s="22"/>
       <c r="J27" s="23"/>
-      <c r="K27" s="22"/>
+      <c r="K27" s="23"/>
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
       <c r="N27" s="0"/>
@@ -21335,22 +21316,22 @@
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="23"/>
       <c r="K28" s="23"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
       <c r="N28" s="0"/>
       <c r="O28" s="0"/>
       <c r="P28" s="0"/>
@@ -22363,1050 +22344,39 @@
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="s">
+    <row r="29" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="0"/>
-      <c r="O29" s="0"/>
-      <c r="P29" s="0"/>
-      <c r="Q29" s="0"/>
-      <c r="R29" s="0"/>
-      <c r="S29" s="0"/>
-      <c r="T29" s="0"/>
-      <c r="U29" s="0"/>
-      <c r="V29" s="0"/>
-      <c r="W29" s="0"/>
-      <c r="X29" s="0"/>
-      <c r="Y29" s="0"/>
-      <c r="Z29" s="0"/>
-      <c r="AA29" s="0"/>
-      <c r="AB29" s="0"/>
-      <c r="AC29" s="0"/>
-      <c r="AD29" s="0"/>
-      <c r="AE29" s="0"/>
-      <c r="AF29" s="0"/>
-      <c r="AG29" s="0"/>
-      <c r="AH29" s="0"/>
-      <c r="AI29" s="0"/>
-      <c r="AJ29" s="0"/>
-      <c r="AK29" s="0"/>
-      <c r="AL29" s="0"/>
-      <c r="AM29" s="0"/>
-      <c r="AN29" s="0"/>
-      <c r="AO29" s="0"/>
-      <c r="AP29" s="0"/>
-      <c r="AQ29" s="0"/>
-      <c r="AR29" s="0"/>
-      <c r="AS29" s="0"/>
-      <c r="AT29" s="0"/>
-      <c r="AU29" s="0"/>
-      <c r="AV29" s="0"/>
-      <c r="AW29" s="0"/>
-      <c r="AX29" s="0"/>
-      <c r="AY29" s="0"/>
-      <c r="AZ29" s="0"/>
-      <c r="BA29" s="0"/>
-      <c r="BB29" s="0"/>
-      <c r="BC29" s="0"/>
-      <c r="BD29" s="0"/>
-      <c r="BE29" s="0"/>
-      <c r="BF29" s="0"/>
-      <c r="BG29" s="0"/>
-      <c r="BH29" s="0"/>
-      <c r="BI29" s="0"/>
-      <c r="BJ29" s="0"/>
-      <c r="BK29" s="0"/>
-      <c r="BL29" s="0"/>
-      <c r="BM29" s="0"/>
-      <c r="BN29" s="0"/>
-      <c r="BO29" s="0"/>
-      <c r="BP29" s="0"/>
-      <c r="BQ29" s="0"/>
-      <c r="BR29" s="0"/>
-      <c r="BS29" s="0"/>
-      <c r="BT29" s="0"/>
-      <c r="BU29" s="0"/>
-      <c r="BV29" s="0"/>
-      <c r="BW29" s="0"/>
-      <c r="BX29" s="0"/>
-      <c r="BY29" s="0"/>
-      <c r="BZ29" s="0"/>
-      <c r="CA29" s="0"/>
-      <c r="CB29" s="0"/>
-      <c r="CC29" s="0"/>
-      <c r="CD29" s="0"/>
-      <c r="CE29" s="0"/>
-      <c r="CF29" s="0"/>
-      <c r="CG29" s="0"/>
-      <c r="CH29" s="0"/>
-      <c r="CI29" s="0"/>
-      <c r="CJ29" s="0"/>
-      <c r="CK29" s="0"/>
-      <c r="CL29" s="0"/>
-      <c r="CM29" s="0"/>
-      <c r="CN29" s="0"/>
-      <c r="CO29" s="0"/>
-      <c r="CP29" s="0"/>
-      <c r="CQ29" s="0"/>
-      <c r="CR29" s="0"/>
-      <c r="CS29" s="0"/>
-      <c r="CT29" s="0"/>
-      <c r="CU29" s="0"/>
-      <c r="CV29" s="0"/>
-      <c r="CW29" s="0"/>
-      <c r="CX29" s="0"/>
-      <c r="CY29" s="0"/>
-      <c r="CZ29" s="0"/>
-      <c r="DA29" s="0"/>
-      <c r="DB29" s="0"/>
-      <c r="DC29" s="0"/>
-      <c r="DD29" s="0"/>
-      <c r="DE29" s="0"/>
-      <c r="DF29" s="0"/>
-      <c r="DG29" s="0"/>
-      <c r="DH29" s="0"/>
-      <c r="DI29" s="0"/>
-      <c r="DJ29" s="0"/>
-      <c r="DK29" s="0"/>
-      <c r="DL29" s="0"/>
-      <c r="DM29" s="0"/>
-      <c r="DN29" s="0"/>
-      <c r="DO29" s="0"/>
-      <c r="DP29" s="0"/>
-      <c r="DQ29" s="0"/>
-      <c r="DR29" s="0"/>
-      <c r="DS29" s="0"/>
-      <c r="DT29" s="0"/>
-      <c r="DU29" s="0"/>
-      <c r="DV29" s="0"/>
-      <c r="DW29" s="0"/>
-      <c r="DX29" s="0"/>
-      <c r="DY29" s="0"/>
-      <c r="DZ29" s="0"/>
-      <c r="EA29" s="0"/>
-      <c r="EB29" s="0"/>
-      <c r="EC29" s="0"/>
-      <c r="ED29" s="0"/>
-      <c r="EE29" s="0"/>
-      <c r="EF29" s="0"/>
-      <c r="EG29" s="0"/>
-      <c r="EH29" s="0"/>
-      <c r="EI29" s="0"/>
-      <c r="EJ29" s="0"/>
-      <c r="EK29" s="0"/>
-      <c r="EL29" s="0"/>
-      <c r="EM29" s="0"/>
-      <c r="EN29" s="0"/>
-      <c r="EO29" s="0"/>
-      <c r="EP29" s="0"/>
-      <c r="EQ29" s="0"/>
-      <c r="ER29" s="0"/>
-      <c r="ES29" s="0"/>
-      <c r="ET29" s="0"/>
-      <c r="EU29" s="0"/>
-      <c r="EV29" s="0"/>
-      <c r="EW29" s="0"/>
-      <c r="EX29" s="0"/>
-      <c r="EY29" s="0"/>
-      <c r="EZ29" s="0"/>
-      <c r="FA29" s="0"/>
-      <c r="FB29" s="0"/>
-      <c r="FC29" s="0"/>
-      <c r="FD29" s="0"/>
-      <c r="FE29" s="0"/>
-      <c r="FF29" s="0"/>
-      <c r="FG29" s="0"/>
-      <c r="FH29" s="0"/>
-      <c r="FI29" s="0"/>
-      <c r="FJ29" s="0"/>
-      <c r="FK29" s="0"/>
-      <c r="FL29" s="0"/>
-      <c r="FM29" s="0"/>
-      <c r="FN29" s="0"/>
-      <c r="FO29" s="0"/>
-      <c r="FP29" s="0"/>
-      <c r="FQ29" s="0"/>
-      <c r="FR29" s="0"/>
-      <c r="FS29" s="0"/>
-      <c r="FT29" s="0"/>
-      <c r="FU29" s="0"/>
-      <c r="FV29" s="0"/>
-      <c r="FW29" s="0"/>
-      <c r="FX29" s="0"/>
-      <c r="FY29" s="0"/>
-      <c r="FZ29" s="0"/>
-      <c r="GA29" s="0"/>
-      <c r="GB29" s="0"/>
-      <c r="GC29" s="0"/>
-      <c r="GD29" s="0"/>
-      <c r="GE29" s="0"/>
-      <c r="GF29" s="0"/>
-      <c r="GG29" s="0"/>
-      <c r="GH29" s="0"/>
-      <c r="GI29" s="0"/>
-      <c r="GJ29" s="0"/>
-      <c r="GK29" s="0"/>
-      <c r="GL29" s="0"/>
-      <c r="GM29" s="0"/>
-      <c r="GN29" s="0"/>
-      <c r="GO29" s="0"/>
-      <c r="GP29" s="0"/>
-      <c r="GQ29" s="0"/>
-      <c r="GR29" s="0"/>
-      <c r="GS29" s="0"/>
-      <c r="GT29" s="0"/>
-      <c r="GU29" s="0"/>
-      <c r="GV29" s="0"/>
-      <c r="GW29" s="0"/>
-      <c r="GX29" s="0"/>
-      <c r="GY29" s="0"/>
-      <c r="GZ29" s="0"/>
-      <c r="HA29" s="0"/>
-      <c r="HB29" s="0"/>
-      <c r="HC29" s="0"/>
-      <c r="HD29" s="0"/>
-      <c r="HE29" s="0"/>
-      <c r="HF29" s="0"/>
-      <c r="HG29" s="0"/>
-      <c r="HH29" s="0"/>
-      <c r="HI29" s="0"/>
-      <c r="HJ29" s="0"/>
-      <c r="HK29" s="0"/>
-      <c r="HL29" s="0"/>
-      <c r="HM29" s="0"/>
-      <c r="HN29" s="0"/>
-      <c r="HO29" s="0"/>
-      <c r="HP29" s="0"/>
-      <c r="HQ29" s="0"/>
-      <c r="HR29" s="0"/>
-      <c r="HS29" s="0"/>
-      <c r="HT29" s="0"/>
-      <c r="HU29" s="0"/>
-      <c r="HV29" s="0"/>
-      <c r="HW29" s="0"/>
-      <c r="HX29" s="0"/>
-      <c r="HY29" s="0"/>
-      <c r="HZ29" s="0"/>
-      <c r="IA29" s="0"/>
-      <c r="IB29" s="0"/>
-      <c r="IC29" s="0"/>
-      <c r="ID29" s="0"/>
-      <c r="IE29" s="0"/>
-      <c r="IF29" s="0"/>
-      <c r="IG29" s="0"/>
-      <c r="IH29" s="0"/>
-      <c r="II29" s="0"/>
-      <c r="IJ29" s="0"/>
-      <c r="IK29" s="0"/>
-      <c r="IL29" s="0"/>
-      <c r="IM29" s="0"/>
-      <c r="IN29" s="0"/>
-      <c r="IO29" s="0"/>
-      <c r="IP29" s="0"/>
-      <c r="IQ29" s="0"/>
-      <c r="IR29" s="0"/>
-      <c r="IS29" s="0"/>
-      <c r="IT29" s="0"/>
-      <c r="IU29" s="0"/>
-      <c r="IV29" s="0"/>
-      <c r="IW29" s="0"/>
-      <c r="IX29" s="0"/>
-      <c r="IY29" s="0"/>
-      <c r="IZ29" s="0"/>
-      <c r="JA29" s="0"/>
-      <c r="JB29" s="0"/>
-      <c r="JC29" s="0"/>
-      <c r="JD29" s="0"/>
-      <c r="JE29" s="0"/>
-      <c r="JF29" s="0"/>
-      <c r="JG29" s="0"/>
-      <c r="JH29" s="0"/>
-      <c r="JI29" s="0"/>
-      <c r="JJ29" s="0"/>
-      <c r="JK29" s="0"/>
-      <c r="JL29" s="0"/>
-      <c r="JM29" s="0"/>
-      <c r="JN29" s="0"/>
-      <c r="JO29" s="0"/>
-      <c r="JP29" s="0"/>
-      <c r="JQ29" s="0"/>
-      <c r="JR29" s="0"/>
-      <c r="JS29" s="0"/>
-      <c r="JT29" s="0"/>
-      <c r="JU29" s="0"/>
-      <c r="JV29" s="0"/>
-      <c r="JW29" s="0"/>
-      <c r="JX29" s="0"/>
-      <c r="JY29" s="0"/>
-      <c r="JZ29" s="0"/>
-      <c r="KA29" s="0"/>
-      <c r="KB29" s="0"/>
-      <c r="KC29" s="0"/>
-      <c r="KD29" s="0"/>
-      <c r="KE29" s="0"/>
-      <c r="KF29" s="0"/>
-      <c r="KG29" s="0"/>
-      <c r="KH29" s="0"/>
-      <c r="KI29" s="0"/>
-      <c r="KJ29" s="0"/>
-      <c r="KK29" s="0"/>
-      <c r="KL29" s="0"/>
-      <c r="KM29" s="0"/>
-      <c r="KN29" s="0"/>
-      <c r="KO29" s="0"/>
-      <c r="KP29" s="0"/>
-      <c r="KQ29" s="0"/>
-      <c r="KR29" s="0"/>
-      <c r="KS29" s="0"/>
-      <c r="KT29" s="0"/>
-      <c r="KU29" s="0"/>
-      <c r="KV29" s="0"/>
-      <c r="KW29" s="0"/>
-      <c r="KX29" s="0"/>
-      <c r="KY29" s="0"/>
-      <c r="KZ29" s="0"/>
-      <c r="LA29" s="0"/>
-      <c r="LB29" s="0"/>
-      <c r="LC29" s="0"/>
-      <c r="LD29" s="0"/>
-      <c r="LE29" s="0"/>
-      <c r="LF29" s="0"/>
-      <c r="LG29" s="0"/>
-      <c r="LH29" s="0"/>
-      <c r="LI29" s="0"/>
-      <c r="LJ29" s="0"/>
-      <c r="LK29" s="0"/>
-      <c r="LL29" s="0"/>
-      <c r="LM29" s="0"/>
-      <c r="LN29" s="0"/>
-      <c r="LO29" s="0"/>
-      <c r="LP29" s="0"/>
-      <c r="LQ29" s="0"/>
-      <c r="LR29" s="0"/>
-      <c r="LS29" s="0"/>
-      <c r="LT29" s="0"/>
-      <c r="LU29" s="0"/>
-      <c r="LV29" s="0"/>
-      <c r="LW29" s="0"/>
-      <c r="LX29" s="0"/>
-      <c r="LY29" s="0"/>
-      <c r="LZ29" s="0"/>
-      <c r="MA29" s="0"/>
-      <c r="MB29" s="0"/>
-      <c r="MC29" s="0"/>
-      <c r="MD29" s="0"/>
-      <c r="ME29" s="0"/>
-      <c r="MF29" s="0"/>
-      <c r="MG29" s="0"/>
-      <c r="MH29" s="0"/>
-      <c r="MI29" s="0"/>
-      <c r="MJ29" s="0"/>
-      <c r="MK29" s="0"/>
-      <c r="ML29" s="0"/>
-      <c r="MM29" s="0"/>
-      <c r="MN29" s="0"/>
-      <c r="MO29" s="0"/>
-      <c r="MP29" s="0"/>
-      <c r="MQ29" s="0"/>
-      <c r="MR29" s="0"/>
-      <c r="MS29" s="0"/>
-      <c r="MT29" s="0"/>
-      <c r="MU29" s="0"/>
-      <c r="MV29" s="0"/>
-      <c r="MW29" s="0"/>
-      <c r="MX29" s="0"/>
-      <c r="MY29" s="0"/>
-      <c r="MZ29" s="0"/>
-      <c r="NA29" s="0"/>
-      <c r="NB29" s="0"/>
-      <c r="NC29" s="0"/>
-      <c r="ND29" s="0"/>
-      <c r="NE29" s="0"/>
-      <c r="NF29" s="0"/>
-      <c r="NG29" s="0"/>
-      <c r="NH29" s="0"/>
-      <c r="NI29" s="0"/>
-      <c r="NJ29" s="0"/>
-      <c r="NK29" s="0"/>
-      <c r="NL29" s="0"/>
-      <c r="NM29" s="0"/>
-      <c r="NN29" s="0"/>
-      <c r="NO29" s="0"/>
-      <c r="NP29" s="0"/>
-      <c r="NQ29" s="0"/>
-      <c r="NR29" s="0"/>
-      <c r="NS29" s="0"/>
-      <c r="NT29" s="0"/>
-      <c r="NU29" s="0"/>
-      <c r="NV29" s="0"/>
-      <c r="NW29" s="0"/>
-      <c r="NX29" s="0"/>
-      <c r="NY29" s="0"/>
-      <c r="NZ29" s="0"/>
-      <c r="OA29" s="0"/>
-      <c r="OB29" s="0"/>
-      <c r="OC29" s="0"/>
-      <c r="OD29" s="0"/>
-      <c r="OE29" s="0"/>
-      <c r="OF29" s="0"/>
-      <c r="OG29" s="0"/>
-      <c r="OH29" s="0"/>
-      <c r="OI29" s="0"/>
-      <c r="OJ29" s="0"/>
-      <c r="OK29" s="0"/>
-      <c r="OL29" s="0"/>
-      <c r="OM29" s="0"/>
-      <c r="ON29" s="0"/>
-      <c r="OO29" s="0"/>
-      <c r="OP29" s="0"/>
-      <c r="OQ29" s="0"/>
-      <c r="OR29" s="0"/>
-      <c r="OS29" s="0"/>
-      <c r="OT29" s="0"/>
-      <c r="OU29" s="0"/>
-      <c r="OV29" s="0"/>
-      <c r="OW29" s="0"/>
-      <c r="OX29" s="0"/>
-      <c r="OY29" s="0"/>
-      <c r="OZ29" s="0"/>
-      <c r="PA29" s="0"/>
-      <c r="PB29" s="0"/>
-      <c r="PC29" s="0"/>
-      <c r="PD29" s="0"/>
-      <c r="PE29" s="0"/>
-      <c r="PF29" s="0"/>
-      <c r="PG29" s="0"/>
-      <c r="PH29" s="0"/>
-      <c r="PI29" s="0"/>
-      <c r="PJ29" s="0"/>
-      <c r="PK29" s="0"/>
-      <c r="PL29" s="0"/>
-      <c r="PM29" s="0"/>
-      <c r="PN29" s="0"/>
-      <c r="PO29" s="0"/>
-      <c r="PP29" s="0"/>
-      <c r="PQ29" s="0"/>
-      <c r="PR29" s="0"/>
-      <c r="PS29" s="0"/>
-      <c r="PT29" s="0"/>
-      <c r="PU29" s="0"/>
-      <c r="PV29" s="0"/>
-      <c r="PW29" s="0"/>
-      <c r="PX29" s="0"/>
-      <c r="PY29" s="0"/>
-      <c r="PZ29" s="0"/>
-      <c r="QA29" s="0"/>
-      <c r="QB29" s="0"/>
-      <c r="QC29" s="0"/>
-      <c r="QD29" s="0"/>
-      <c r="QE29" s="0"/>
-      <c r="QF29" s="0"/>
-      <c r="QG29" s="0"/>
-      <c r="QH29" s="0"/>
-      <c r="QI29" s="0"/>
-      <c r="QJ29" s="0"/>
-      <c r="QK29" s="0"/>
-      <c r="QL29" s="0"/>
-      <c r="QM29" s="0"/>
-      <c r="QN29" s="0"/>
-      <c r="QO29" s="0"/>
-      <c r="QP29" s="0"/>
-      <c r="QQ29" s="0"/>
-      <c r="QR29" s="0"/>
-      <c r="QS29" s="0"/>
-      <c r="QT29" s="0"/>
-      <c r="QU29" s="0"/>
-      <c r="QV29" s="0"/>
-      <c r="QW29" s="0"/>
-      <c r="QX29" s="0"/>
-      <c r="QY29" s="0"/>
-      <c r="QZ29" s="0"/>
-      <c r="RA29" s="0"/>
-      <c r="RB29" s="0"/>
-      <c r="RC29" s="0"/>
-      <c r="RD29" s="0"/>
-      <c r="RE29" s="0"/>
-      <c r="RF29" s="0"/>
-      <c r="RG29" s="0"/>
-      <c r="RH29" s="0"/>
-      <c r="RI29" s="0"/>
-      <c r="RJ29" s="0"/>
-      <c r="RK29" s="0"/>
-      <c r="RL29" s="0"/>
-      <c r="RM29" s="0"/>
-      <c r="RN29" s="0"/>
-      <c r="RO29" s="0"/>
-      <c r="RP29" s="0"/>
-      <c r="RQ29" s="0"/>
-      <c r="RR29" s="0"/>
-      <c r="RS29" s="0"/>
-      <c r="RT29" s="0"/>
-      <c r="RU29" s="0"/>
-      <c r="RV29" s="0"/>
-      <c r="RW29" s="0"/>
-      <c r="RX29" s="0"/>
-      <c r="RY29" s="0"/>
-      <c r="RZ29" s="0"/>
-      <c r="SA29" s="0"/>
-      <c r="SB29" s="0"/>
-      <c r="SC29" s="0"/>
-      <c r="SD29" s="0"/>
-      <c r="SE29" s="0"/>
-      <c r="SF29" s="0"/>
-      <c r="SG29" s="0"/>
-      <c r="SH29" s="0"/>
-      <c r="SI29" s="0"/>
-      <c r="SJ29" s="0"/>
-      <c r="SK29" s="0"/>
-      <c r="SL29" s="0"/>
-      <c r="SM29" s="0"/>
-      <c r="SN29" s="0"/>
-      <c r="SO29" s="0"/>
-      <c r="SP29" s="0"/>
-      <c r="SQ29" s="0"/>
-      <c r="SR29" s="0"/>
-      <c r="SS29" s="0"/>
-      <c r="ST29" s="0"/>
-      <c r="SU29" s="0"/>
-      <c r="SV29" s="0"/>
-      <c r="SW29" s="0"/>
-      <c r="SX29" s="0"/>
-      <c r="SY29" s="0"/>
-      <c r="SZ29" s="0"/>
-      <c r="TA29" s="0"/>
-      <c r="TB29" s="0"/>
-      <c r="TC29" s="0"/>
-      <c r="TD29" s="0"/>
-      <c r="TE29" s="0"/>
-      <c r="TF29" s="0"/>
-      <c r="TG29" s="0"/>
-      <c r="TH29" s="0"/>
-      <c r="TI29" s="0"/>
-      <c r="TJ29" s="0"/>
-      <c r="TK29" s="0"/>
-      <c r="TL29" s="0"/>
-      <c r="TM29" s="0"/>
-      <c r="TN29" s="0"/>
-      <c r="TO29" s="0"/>
-      <c r="TP29" s="0"/>
-      <c r="TQ29" s="0"/>
-      <c r="TR29" s="0"/>
-      <c r="TS29" s="0"/>
-      <c r="TT29" s="0"/>
-      <c r="TU29" s="0"/>
-      <c r="TV29" s="0"/>
-      <c r="TW29" s="0"/>
-      <c r="TX29" s="0"/>
-      <c r="TY29" s="0"/>
-      <c r="TZ29" s="0"/>
-      <c r="UA29" s="0"/>
-      <c r="UB29" s="0"/>
-      <c r="UC29" s="0"/>
-      <c r="UD29" s="0"/>
-      <c r="UE29" s="0"/>
-      <c r="UF29" s="0"/>
-      <c r="UG29" s="0"/>
-      <c r="UH29" s="0"/>
-      <c r="UI29" s="0"/>
-      <c r="UJ29" s="0"/>
-      <c r="UK29" s="0"/>
-      <c r="UL29" s="0"/>
-      <c r="UM29" s="0"/>
-      <c r="UN29" s="0"/>
-      <c r="UO29" s="0"/>
-      <c r="UP29" s="0"/>
-      <c r="UQ29" s="0"/>
-      <c r="UR29" s="0"/>
-      <c r="US29" s="0"/>
-      <c r="UT29" s="0"/>
-      <c r="UU29" s="0"/>
-      <c r="UV29" s="0"/>
-      <c r="UW29" s="0"/>
-      <c r="UX29" s="0"/>
-      <c r="UY29" s="0"/>
-      <c r="UZ29" s="0"/>
-      <c r="VA29" s="0"/>
-      <c r="VB29" s="0"/>
-      <c r="VC29" s="0"/>
-      <c r="VD29" s="0"/>
-      <c r="VE29" s="0"/>
-      <c r="VF29" s="0"/>
-      <c r="VG29" s="0"/>
-      <c r="VH29" s="0"/>
-      <c r="VI29" s="0"/>
-      <c r="VJ29" s="0"/>
-      <c r="VK29" s="0"/>
-      <c r="VL29" s="0"/>
-      <c r="VM29" s="0"/>
-      <c r="VN29" s="0"/>
-      <c r="VO29" s="0"/>
-      <c r="VP29" s="0"/>
-      <c r="VQ29" s="0"/>
-      <c r="VR29" s="0"/>
-      <c r="VS29" s="0"/>
-      <c r="VT29" s="0"/>
-      <c r="VU29" s="0"/>
-      <c r="VV29" s="0"/>
-      <c r="VW29" s="0"/>
-      <c r="VX29" s="0"/>
-      <c r="VY29" s="0"/>
-      <c r="VZ29" s="0"/>
-      <c r="WA29" s="0"/>
-      <c r="WB29" s="0"/>
-      <c r="WC29" s="0"/>
-      <c r="WD29" s="0"/>
-      <c r="WE29" s="0"/>
-      <c r="WF29" s="0"/>
-      <c r="WG29" s="0"/>
-      <c r="WH29" s="0"/>
-      <c r="WI29" s="0"/>
-      <c r="WJ29" s="0"/>
-      <c r="WK29" s="0"/>
-      <c r="WL29" s="0"/>
-      <c r="WM29" s="0"/>
-      <c r="WN29" s="0"/>
-      <c r="WO29" s="0"/>
-      <c r="WP29" s="0"/>
-      <c r="WQ29" s="0"/>
-      <c r="WR29" s="0"/>
-      <c r="WS29" s="0"/>
-      <c r="WT29" s="0"/>
-      <c r="WU29" s="0"/>
-      <c r="WV29" s="0"/>
-      <c r="WW29" s="0"/>
-      <c r="WX29" s="0"/>
-      <c r="WY29" s="0"/>
-      <c r="WZ29" s="0"/>
-      <c r="XA29" s="0"/>
-      <c r="XB29" s="0"/>
-      <c r="XC29" s="0"/>
-      <c r="XD29" s="0"/>
-      <c r="XE29" s="0"/>
-      <c r="XF29" s="0"/>
-      <c r="XG29" s="0"/>
-      <c r="XH29" s="0"/>
-      <c r="XI29" s="0"/>
-      <c r="XJ29" s="0"/>
-      <c r="XK29" s="0"/>
-      <c r="XL29" s="0"/>
-      <c r="XM29" s="0"/>
-      <c r="XN29" s="0"/>
-      <c r="XO29" s="0"/>
-      <c r="XP29" s="0"/>
-      <c r="XQ29" s="0"/>
-      <c r="XR29" s="0"/>
-      <c r="XS29" s="0"/>
-      <c r="XT29" s="0"/>
-      <c r="XU29" s="0"/>
-      <c r="XV29" s="0"/>
-      <c r="XW29" s="0"/>
-      <c r="XX29" s="0"/>
-      <c r="XY29" s="0"/>
-      <c r="XZ29" s="0"/>
-      <c r="YA29" s="0"/>
-      <c r="YB29" s="0"/>
-      <c r="YC29" s="0"/>
-      <c r="YD29" s="0"/>
-      <c r="YE29" s="0"/>
-      <c r="YF29" s="0"/>
-      <c r="YG29" s="0"/>
-      <c r="YH29" s="0"/>
-      <c r="YI29" s="0"/>
-      <c r="YJ29" s="0"/>
-      <c r="YK29" s="0"/>
-      <c r="YL29" s="0"/>
-      <c r="YM29" s="0"/>
-      <c r="YN29" s="0"/>
-      <c r="YO29" s="0"/>
-      <c r="YP29" s="0"/>
-      <c r="YQ29" s="0"/>
-      <c r="YR29" s="0"/>
-      <c r="YS29" s="0"/>
-      <c r="YT29" s="0"/>
-      <c r="YU29" s="0"/>
-      <c r="YV29" s="0"/>
-      <c r="YW29" s="0"/>
-      <c r="YX29" s="0"/>
-      <c r="YY29" s="0"/>
-      <c r="YZ29" s="0"/>
-      <c r="ZA29" s="0"/>
-      <c r="ZB29" s="0"/>
-      <c r="ZC29" s="0"/>
-      <c r="ZD29" s="0"/>
-      <c r="ZE29" s="0"/>
-      <c r="ZF29" s="0"/>
-      <c r="ZG29" s="0"/>
-      <c r="ZH29" s="0"/>
-      <c r="ZI29" s="0"/>
-      <c r="ZJ29" s="0"/>
-      <c r="ZK29" s="0"/>
-      <c r="ZL29" s="0"/>
-      <c r="ZM29" s="0"/>
-      <c r="ZN29" s="0"/>
-      <c r="ZO29" s="0"/>
-      <c r="ZP29" s="0"/>
-      <c r="ZQ29" s="0"/>
-      <c r="ZR29" s="0"/>
-      <c r="ZS29" s="0"/>
-      <c r="ZT29" s="0"/>
-      <c r="ZU29" s="0"/>
-      <c r="ZV29" s="0"/>
-      <c r="ZW29" s="0"/>
-      <c r="ZX29" s="0"/>
-      <c r="ZY29" s="0"/>
-      <c r="ZZ29" s="0"/>
-      <c r="AAA29" s="0"/>
-      <c r="AAB29" s="0"/>
-      <c r="AAC29" s="0"/>
-      <c r="AAD29" s="0"/>
-      <c r="AAE29" s="0"/>
-      <c r="AAF29" s="0"/>
-      <c r="AAG29" s="0"/>
-      <c r="AAH29" s="0"/>
-      <c r="AAI29" s="0"/>
-      <c r="AAJ29" s="0"/>
-      <c r="AAK29" s="0"/>
-      <c r="AAL29" s="0"/>
-      <c r="AAM29" s="0"/>
-      <c r="AAN29" s="0"/>
-      <c r="AAO29" s="0"/>
-      <c r="AAP29" s="0"/>
-      <c r="AAQ29" s="0"/>
-      <c r="AAR29" s="0"/>
-      <c r="AAS29" s="0"/>
-      <c r="AAT29" s="0"/>
-      <c r="AAU29" s="0"/>
-      <c r="AAV29" s="0"/>
-      <c r="AAW29" s="0"/>
-      <c r="AAX29" s="0"/>
-      <c r="AAY29" s="0"/>
-      <c r="AAZ29" s="0"/>
-      <c r="ABA29" s="0"/>
-      <c r="ABB29" s="0"/>
-      <c r="ABC29" s="0"/>
-      <c r="ABD29" s="0"/>
-      <c r="ABE29" s="0"/>
-      <c r="ABF29" s="0"/>
-      <c r="ABG29" s="0"/>
-      <c r="ABH29" s="0"/>
-      <c r="ABI29" s="0"/>
-      <c r="ABJ29" s="0"/>
-      <c r="ABK29" s="0"/>
-      <c r="ABL29" s="0"/>
-      <c r="ABM29" s="0"/>
-      <c r="ABN29" s="0"/>
-      <c r="ABO29" s="0"/>
-      <c r="ABP29" s="0"/>
-      <c r="ABQ29" s="0"/>
-      <c r="ABR29" s="0"/>
-      <c r="ABS29" s="0"/>
-      <c r="ABT29" s="0"/>
-      <c r="ABU29" s="0"/>
-      <c r="ABV29" s="0"/>
-      <c r="ABW29" s="0"/>
-      <c r="ABX29" s="0"/>
-      <c r="ABY29" s="0"/>
-      <c r="ABZ29" s="0"/>
-      <c r="ACA29" s="0"/>
-      <c r="ACB29" s="0"/>
-      <c r="ACC29" s="0"/>
-      <c r="ACD29" s="0"/>
-      <c r="ACE29" s="0"/>
-      <c r="ACF29" s="0"/>
-      <c r="ACG29" s="0"/>
-      <c r="ACH29" s="0"/>
-      <c r="ACI29" s="0"/>
-      <c r="ACJ29" s="0"/>
-      <c r="ACK29" s="0"/>
-      <c r="ACL29" s="0"/>
-      <c r="ACM29" s="0"/>
-      <c r="ACN29" s="0"/>
-      <c r="ACO29" s="0"/>
-      <c r="ACP29" s="0"/>
-      <c r="ACQ29" s="0"/>
-      <c r="ACR29" s="0"/>
-      <c r="ACS29" s="0"/>
-      <c r="ACT29" s="0"/>
-      <c r="ACU29" s="0"/>
-      <c r="ACV29" s="0"/>
-      <c r="ACW29" s="0"/>
-      <c r="ACX29" s="0"/>
-      <c r="ACY29" s="0"/>
-      <c r="ACZ29" s="0"/>
-      <c r="ADA29" s="0"/>
-      <c r="ADB29" s="0"/>
-      <c r="ADC29" s="0"/>
-      <c r="ADD29" s="0"/>
-      <c r="ADE29" s="0"/>
-      <c r="ADF29" s="0"/>
-      <c r="ADG29" s="0"/>
-      <c r="ADH29" s="0"/>
-      <c r="ADI29" s="0"/>
-      <c r="ADJ29" s="0"/>
-      <c r="ADK29" s="0"/>
-      <c r="ADL29" s="0"/>
-      <c r="ADM29" s="0"/>
-      <c r="ADN29" s="0"/>
-      <c r="ADO29" s="0"/>
-      <c r="ADP29" s="0"/>
-      <c r="ADQ29" s="0"/>
-      <c r="ADR29" s="0"/>
-      <c r="ADS29" s="0"/>
-      <c r="ADT29" s="0"/>
-      <c r="ADU29" s="0"/>
-      <c r="ADV29" s="0"/>
-      <c r="ADW29" s="0"/>
-      <c r="ADX29" s="0"/>
-      <c r="ADY29" s="0"/>
-      <c r="ADZ29" s="0"/>
-      <c r="AEA29" s="0"/>
-      <c r="AEB29" s="0"/>
-      <c r="AEC29" s="0"/>
-      <c r="AED29" s="0"/>
-      <c r="AEE29" s="0"/>
-      <c r="AEF29" s="0"/>
-      <c r="AEG29" s="0"/>
-      <c r="AEH29" s="0"/>
-      <c r="AEI29" s="0"/>
-      <c r="AEJ29" s="0"/>
-      <c r="AEK29" s="0"/>
-      <c r="AEL29" s="0"/>
-      <c r="AEM29" s="0"/>
-      <c r="AEN29" s="0"/>
-      <c r="AEO29" s="0"/>
-      <c r="AEP29" s="0"/>
-      <c r="AEQ29" s="0"/>
-      <c r="AER29" s="0"/>
-      <c r="AES29" s="0"/>
-      <c r="AET29" s="0"/>
-      <c r="AEU29" s="0"/>
-      <c r="AEV29" s="0"/>
-      <c r="AEW29" s="0"/>
-      <c r="AEX29" s="0"/>
-      <c r="AEY29" s="0"/>
-      <c r="AEZ29" s="0"/>
-      <c r="AFA29" s="0"/>
-      <c r="AFB29" s="0"/>
-      <c r="AFC29" s="0"/>
-      <c r="AFD29" s="0"/>
-      <c r="AFE29" s="0"/>
-      <c r="AFF29" s="0"/>
-      <c r="AFG29" s="0"/>
-      <c r="AFH29" s="0"/>
-      <c r="AFI29" s="0"/>
-      <c r="AFJ29" s="0"/>
-      <c r="AFK29" s="0"/>
-      <c r="AFL29" s="0"/>
-      <c r="AFM29" s="0"/>
-      <c r="AFN29" s="0"/>
-      <c r="AFO29" s="0"/>
-      <c r="AFP29" s="0"/>
-      <c r="AFQ29" s="0"/>
-      <c r="AFR29" s="0"/>
-      <c r="AFS29" s="0"/>
-      <c r="AFT29" s="0"/>
-      <c r="AFU29" s="0"/>
-      <c r="AFV29" s="0"/>
-      <c r="AFW29" s="0"/>
-      <c r="AFX29" s="0"/>
-      <c r="AFY29" s="0"/>
-      <c r="AFZ29" s="0"/>
-      <c r="AGA29" s="0"/>
-      <c r="AGB29" s="0"/>
-      <c r="AGC29" s="0"/>
-      <c r="AGD29" s="0"/>
-      <c r="AGE29" s="0"/>
-      <c r="AGF29" s="0"/>
-      <c r="AGG29" s="0"/>
-      <c r="AGH29" s="0"/>
-      <c r="AGI29" s="0"/>
-      <c r="AGJ29" s="0"/>
-      <c r="AGK29" s="0"/>
-      <c r="AGL29" s="0"/>
-      <c r="AGM29" s="0"/>
-      <c r="AGN29" s="0"/>
-      <c r="AGO29" s="0"/>
-      <c r="AGP29" s="0"/>
-      <c r="AGQ29" s="0"/>
-      <c r="AGR29" s="0"/>
-      <c r="AGS29" s="0"/>
-      <c r="AGT29" s="0"/>
-      <c r="AGU29" s="0"/>
-      <c r="AGV29" s="0"/>
-      <c r="AGW29" s="0"/>
-      <c r="AGX29" s="0"/>
-      <c r="AGY29" s="0"/>
-      <c r="AGZ29" s="0"/>
-      <c r="AHA29" s="0"/>
-      <c r="AHB29" s="0"/>
-      <c r="AHC29" s="0"/>
-      <c r="AHD29" s="0"/>
-      <c r="AHE29" s="0"/>
-      <c r="AHF29" s="0"/>
-      <c r="AHG29" s="0"/>
-      <c r="AHH29" s="0"/>
-      <c r="AHI29" s="0"/>
-      <c r="AHJ29" s="0"/>
-      <c r="AHK29" s="0"/>
-      <c r="AHL29" s="0"/>
-      <c r="AHM29" s="0"/>
-      <c r="AHN29" s="0"/>
-      <c r="AHO29" s="0"/>
-      <c r="AHP29" s="0"/>
-      <c r="AHQ29" s="0"/>
-      <c r="AHR29" s="0"/>
-      <c r="AHS29" s="0"/>
-      <c r="AHT29" s="0"/>
-      <c r="AHU29" s="0"/>
-      <c r="AHV29" s="0"/>
-      <c r="AHW29" s="0"/>
-      <c r="AHX29" s="0"/>
-      <c r="AHY29" s="0"/>
-      <c r="AHZ29" s="0"/>
-      <c r="AIA29" s="0"/>
-      <c r="AIB29" s="0"/>
-      <c r="AIC29" s="0"/>
-      <c r="AID29" s="0"/>
-      <c r="AIE29" s="0"/>
-      <c r="AIF29" s="0"/>
-      <c r="AIG29" s="0"/>
-      <c r="AIH29" s="0"/>
-      <c r="AII29" s="0"/>
-      <c r="AIJ29" s="0"/>
-      <c r="AIK29" s="0"/>
-      <c r="AIL29" s="0"/>
-      <c r="AIM29" s="0"/>
-      <c r="AIN29" s="0"/>
-      <c r="AIO29" s="0"/>
-      <c r="AIP29" s="0"/>
-      <c r="AIQ29" s="0"/>
-      <c r="AIR29" s="0"/>
-      <c r="AIS29" s="0"/>
-      <c r="AIT29" s="0"/>
-      <c r="AIU29" s="0"/>
-      <c r="AIV29" s="0"/>
-      <c r="AIW29" s="0"/>
-      <c r="AIX29" s="0"/>
-      <c r="AIY29" s="0"/>
-      <c r="AIZ29" s="0"/>
-      <c r="AJA29" s="0"/>
-      <c r="AJB29" s="0"/>
-      <c r="AJC29" s="0"/>
-      <c r="AJD29" s="0"/>
-      <c r="AJE29" s="0"/>
-      <c r="AJF29" s="0"/>
-      <c r="AJG29" s="0"/>
-      <c r="AJH29" s="0"/>
-      <c r="AJI29" s="0"/>
-      <c r="AJJ29" s="0"/>
-      <c r="AJK29" s="0"/>
-      <c r="AJL29" s="0"/>
-      <c r="AJM29" s="0"/>
-      <c r="AJN29" s="0"/>
-      <c r="AJO29" s="0"/>
-      <c r="AJP29" s="0"/>
-      <c r="AJQ29" s="0"/>
-      <c r="AJR29" s="0"/>
-      <c r="AJS29" s="0"/>
-      <c r="AJT29" s="0"/>
-      <c r="AJU29" s="0"/>
-      <c r="AJV29" s="0"/>
-      <c r="AJW29" s="0"/>
-      <c r="AJX29" s="0"/>
-      <c r="AJY29" s="0"/>
-      <c r="AJZ29" s="0"/>
-      <c r="AKA29" s="0"/>
-      <c r="AKB29" s="0"/>
-      <c r="AKC29" s="0"/>
-      <c r="AKD29" s="0"/>
-      <c r="AKE29" s="0"/>
-      <c r="AKF29" s="0"/>
-      <c r="AKG29" s="0"/>
-      <c r="AKH29" s="0"/>
-      <c r="AKI29" s="0"/>
-      <c r="AKJ29" s="0"/>
-      <c r="AKK29" s="0"/>
-      <c r="AKL29" s="0"/>
-      <c r="AKM29" s="0"/>
-      <c r="AKN29" s="0"/>
-      <c r="AKO29" s="0"/>
-      <c r="AKP29" s="0"/>
-      <c r="AKQ29" s="0"/>
-      <c r="AKR29" s="0"/>
-      <c r="AKS29" s="0"/>
-      <c r="AKT29" s="0"/>
-      <c r="AKU29" s="0"/>
-      <c r="AKV29" s="0"/>
-      <c r="AKW29" s="0"/>
-      <c r="AKX29" s="0"/>
-      <c r="AKY29" s="0"/>
-      <c r="AKZ29" s="0"/>
-      <c r="ALA29" s="0"/>
-      <c r="ALB29" s="0"/>
-      <c r="ALC29" s="0"/>
-      <c r="ALD29" s="0"/>
-      <c r="ALE29" s="0"/>
-      <c r="ALF29" s="0"/>
-      <c r="ALG29" s="0"/>
-      <c r="ALH29" s="0"/>
-      <c r="ALI29" s="0"/>
-      <c r="ALJ29" s="0"/>
-      <c r="ALK29" s="0"/>
-      <c r="ALL29" s="0"/>
-      <c r="ALM29" s="0"/>
-      <c r="ALN29" s="0"/>
-      <c r="ALO29" s="0"/>
-      <c r="ALP29" s="0"/>
-      <c r="ALQ29" s="0"/>
-      <c r="ALR29" s="0"/>
-      <c r="ALS29" s="0"/>
-      <c r="ALT29" s="0"/>
-      <c r="ALU29" s="0"/>
-      <c r="ALV29" s="0"/>
-      <c r="ALW29" s="0"/>
-      <c r="ALX29" s="0"/>
-      <c r="ALY29" s="0"/>
-      <c r="ALZ29" s="0"/>
-      <c r="AMA29" s="0"/>
-      <c r="AMB29" s="0"/>
-      <c r="AMC29" s="0"/>
-      <c r="AMD29" s="0"/>
-      <c r="AME29" s="0"/>
-      <c r="AMF29" s="0"/>
-      <c r="AMG29" s="0"/>
-      <c r="AMH29" s="0"/>
-      <c r="AMI29" s="0"/>
-      <c r="AMJ29" s="0"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
       <c r="N30" s="0"/>
       <c r="O30" s="0"/>
       <c r="P30" s="0"/>
@@ -24419,30 +23389,1041 @@
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="0"/>
+      <c r="O31" s="0"/>
+      <c r="P31" s="0"/>
+      <c r="Q31" s="0"/>
+      <c r="R31" s="0"/>
+      <c r="S31" s="0"/>
+      <c r="T31" s="0"/>
+      <c r="U31" s="0"/>
+      <c r="V31" s="0"/>
+      <c r="W31" s="0"/>
+      <c r="X31" s="0"/>
+      <c r="Y31" s="0"/>
+      <c r="Z31" s="0"/>
+      <c r="AA31" s="0"/>
+      <c r="AB31" s="0"/>
+      <c r="AC31" s="0"/>
+      <c r="AD31" s="0"/>
+      <c r="AE31" s="0"/>
+      <c r="AF31" s="0"/>
+      <c r="AG31" s="0"/>
+      <c r="AH31" s="0"/>
+      <c r="AI31" s="0"/>
+      <c r="AJ31" s="0"/>
+      <c r="AK31" s="0"/>
+      <c r="AL31" s="0"/>
+      <c r="AM31" s="0"/>
+      <c r="AN31" s="0"/>
+      <c r="AO31" s="0"/>
+      <c r="AP31" s="0"/>
+      <c r="AQ31" s="0"/>
+      <c r="AR31" s="0"/>
+      <c r="AS31" s="0"/>
+      <c r="AT31" s="0"/>
+      <c r="AU31" s="0"/>
+      <c r="AV31" s="0"/>
+      <c r="AW31" s="0"/>
+      <c r="AX31" s="0"/>
+      <c r="AY31" s="0"/>
+      <c r="AZ31" s="0"/>
+      <c r="BA31" s="0"/>
+      <c r="BB31" s="0"/>
+      <c r="BC31" s="0"/>
+      <c r="BD31" s="0"/>
+      <c r="BE31" s="0"/>
+      <c r="BF31" s="0"/>
+      <c r="BG31" s="0"/>
+      <c r="BH31" s="0"/>
+      <c r="BI31" s="0"/>
+      <c r="BJ31" s="0"/>
+      <c r="BK31" s="0"/>
+      <c r="BL31" s="0"/>
+      <c r="BM31" s="0"/>
+      <c r="BN31" s="0"/>
+      <c r="BO31" s="0"/>
+      <c r="BP31" s="0"/>
+      <c r="BQ31" s="0"/>
+      <c r="BR31" s="0"/>
+      <c r="BS31" s="0"/>
+      <c r="BT31" s="0"/>
+      <c r="BU31" s="0"/>
+      <c r="BV31" s="0"/>
+      <c r="BW31" s="0"/>
+      <c r="BX31" s="0"/>
+      <c r="BY31" s="0"/>
+      <c r="BZ31" s="0"/>
+      <c r="CA31" s="0"/>
+      <c r="CB31" s="0"/>
+      <c r="CC31" s="0"/>
+      <c r="CD31" s="0"/>
+      <c r="CE31" s="0"/>
+      <c r="CF31" s="0"/>
+      <c r="CG31" s="0"/>
+      <c r="CH31" s="0"/>
+      <c r="CI31" s="0"/>
+      <c r="CJ31" s="0"/>
+      <c r="CK31" s="0"/>
+      <c r="CL31" s="0"/>
+      <c r="CM31" s="0"/>
+      <c r="CN31" s="0"/>
+      <c r="CO31" s="0"/>
+      <c r="CP31" s="0"/>
+      <c r="CQ31" s="0"/>
+      <c r="CR31" s="0"/>
+      <c r="CS31" s="0"/>
+      <c r="CT31" s="0"/>
+      <c r="CU31" s="0"/>
+      <c r="CV31" s="0"/>
+      <c r="CW31" s="0"/>
+      <c r="CX31" s="0"/>
+      <c r="CY31" s="0"/>
+      <c r="CZ31" s="0"/>
+      <c r="DA31" s="0"/>
+      <c r="DB31" s="0"/>
+      <c r="DC31" s="0"/>
+      <c r="DD31" s="0"/>
+      <c r="DE31" s="0"/>
+      <c r="DF31" s="0"/>
+      <c r="DG31" s="0"/>
+      <c r="DH31" s="0"/>
+      <c r="DI31" s="0"/>
+      <c r="DJ31" s="0"/>
+      <c r="DK31" s="0"/>
+      <c r="DL31" s="0"/>
+      <c r="DM31" s="0"/>
+      <c r="DN31" s="0"/>
+      <c r="DO31" s="0"/>
+      <c r="DP31" s="0"/>
+      <c r="DQ31" s="0"/>
+      <c r="DR31" s="0"/>
+      <c r="DS31" s="0"/>
+      <c r="DT31" s="0"/>
+      <c r="DU31" s="0"/>
+      <c r="DV31" s="0"/>
+      <c r="DW31" s="0"/>
+      <c r="DX31" s="0"/>
+      <c r="DY31" s="0"/>
+      <c r="DZ31" s="0"/>
+      <c r="EA31" s="0"/>
+      <c r="EB31" s="0"/>
+      <c r="EC31" s="0"/>
+      <c r="ED31" s="0"/>
+      <c r="EE31" s="0"/>
+      <c r="EF31" s="0"/>
+      <c r="EG31" s="0"/>
+      <c r="EH31" s="0"/>
+      <c r="EI31" s="0"/>
+      <c r="EJ31" s="0"/>
+      <c r="EK31" s="0"/>
+      <c r="EL31" s="0"/>
+      <c r="EM31" s="0"/>
+      <c r="EN31" s="0"/>
+      <c r="EO31" s="0"/>
+      <c r="EP31" s="0"/>
+      <c r="EQ31" s="0"/>
+      <c r="ER31" s="0"/>
+      <c r="ES31" s="0"/>
+      <c r="ET31" s="0"/>
+      <c r="EU31" s="0"/>
+      <c r="EV31" s="0"/>
+      <c r="EW31" s="0"/>
+      <c r="EX31" s="0"/>
+      <c r="EY31" s="0"/>
+      <c r="EZ31" s="0"/>
+      <c r="FA31" s="0"/>
+      <c r="FB31" s="0"/>
+      <c r="FC31" s="0"/>
+      <c r="FD31" s="0"/>
+      <c r="FE31" s="0"/>
+      <c r="FF31" s="0"/>
+      <c r="FG31" s="0"/>
+      <c r="FH31" s="0"/>
+      <c r="FI31" s="0"/>
+      <c r="FJ31" s="0"/>
+      <c r="FK31" s="0"/>
+      <c r="FL31" s="0"/>
+      <c r="FM31" s="0"/>
+      <c r="FN31" s="0"/>
+      <c r="FO31" s="0"/>
+      <c r="FP31" s="0"/>
+      <c r="FQ31" s="0"/>
+      <c r="FR31" s="0"/>
+      <c r="FS31" s="0"/>
+      <c r="FT31" s="0"/>
+      <c r="FU31" s="0"/>
+      <c r="FV31" s="0"/>
+      <c r="FW31" s="0"/>
+      <c r="FX31" s="0"/>
+      <c r="FY31" s="0"/>
+      <c r="FZ31" s="0"/>
+      <c r="GA31" s="0"/>
+      <c r="GB31" s="0"/>
+      <c r="GC31" s="0"/>
+      <c r="GD31" s="0"/>
+      <c r="GE31" s="0"/>
+      <c r="GF31" s="0"/>
+      <c r="GG31" s="0"/>
+      <c r="GH31" s="0"/>
+      <c r="GI31" s="0"/>
+      <c r="GJ31" s="0"/>
+      <c r="GK31" s="0"/>
+      <c r="GL31" s="0"/>
+      <c r="GM31" s="0"/>
+      <c r="GN31" s="0"/>
+      <c r="GO31" s="0"/>
+      <c r="GP31" s="0"/>
+      <c r="GQ31" s="0"/>
+      <c r="GR31" s="0"/>
+      <c r="GS31" s="0"/>
+      <c r="GT31" s="0"/>
+      <c r="GU31" s="0"/>
+      <c r="GV31" s="0"/>
+      <c r="GW31" s="0"/>
+      <c r="GX31" s="0"/>
+      <c r="GY31" s="0"/>
+      <c r="GZ31" s="0"/>
+      <c r="HA31" s="0"/>
+      <c r="HB31" s="0"/>
+      <c r="HC31" s="0"/>
+      <c r="HD31" s="0"/>
+      <c r="HE31" s="0"/>
+      <c r="HF31" s="0"/>
+      <c r="HG31" s="0"/>
+      <c r="HH31" s="0"/>
+      <c r="HI31" s="0"/>
+      <c r="HJ31" s="0"/>
+      <c r="HK31" s="0"/>
+      <c r="HL31" s="0"/>
+      <c r="HM31" s="0"/>
+      <c r="HN31" s="0"/>
+      <c r="HO31" s="0"/>
+      <c r="HP31" s="0"/>
+      <c r="HQ31" s="0"/>
+      <c r="HR31" s="0"/>
+      <c r="HS31" s="0"/>
+      <c r="HT31" s="0"/>
+      <c r="HU31" s="0"/>
+      <c r="HV31" s="0"/>
+      <c r="HW31" s="0"/>
+      <c r="HX31" s="0"/>
+      <c r="HY31" s="0"/>
+      <c r="HZ31" s="0"/>
+      <c r="IA31" s="0"/>
+      <c r="IB31" s="0"/>
+      <c r="IC31" s="0"/>
+      <c r="ID31" s="0"/>
+      <c r="IE31" s="0"/>
+      <c r="IF31" s="0"/>
+      <c r="IG31" s="0"/>
+      <c r="IH31" s="0"/>
+      <c r="II31" s="0"/>
+      <c r="IJ31" s="0"/>
+      <c r="IK31" s="0"/>
+      <c r="IL31" s="0"/>
+      <c r="IM31" s="0"/>
+      <c r="IN31" s="0"/>
+      <c r="IO31" s="0"/>
+      <c r="IP31" s="0"/>
+      <c r="IQ31" s="0"/>
+      <c r="IR31" s="0"/>
+      <c r="IS31" s="0"/>
+      <c r="IT31" s="0"/>
+      <c r="IU31" s="0"/>
+      <c r="IV31" s="0"/>
+      <c r="IW31" s="0"/>
+      <c r="IX31" s="0"/>
+      <c r="IY31" s="0"/>
+      <c r="IZ31" s="0"/>
+      <c r="JA31" s="0"/>
+      <c r="JB31" s="0"/>
+      <c r="JC31" s="0"/>
+      <c r="JD31" s="0"/>
+      <c r="JE31" s="0"/>
+      <c r="JF31" s="0"/>
+      <c r="JG31" s="0"/>
+      <c r="JH31" s="0"/>
+      <c r="JI31" s="0"/>
+      <c r="JJ31" s="0"/>
+      <c r="JK31" s="0"/>
+      <c r="JL31" s="0"/>
+      <c r="JM31" s="0"/>
+      <c r="JN31" s="0"/>
+      <c r="JO31" s="0"/>
+      <c r="JP31" s="0"/>
+      <c r="JQ31" s="0"/>
+      <c r="JR31" s="0"/>
+      <c r="JS31" s="0"/>
+      <c r="JT31" s="0"/>
+      <c r="JU31" s="0"/>
+      <c r="JV31" s="0"/>
+      <c r="JW31" s="0"/>
+      <c r="JX31" s="0"/>
+      <c r="JY31" s="0"/>
+      <c r="JZ31" s="0"/>
+      <c r="KA31" s="0"/>
+      <c r="KB31" s="0"/>
+      <c r="KC31" s="0"/>
+      <c r="KD31" s="0"/>
+      <c r="KE31" s="0"/>
+      <c r="KF31" s="0"/>
+      <c r="KG31" s="0"/>
+      <c r="KH31" s="0"/>
+      <c r="KI31" s="0"/>
+      <c r="KJ31" s="0"/>
+      <c r="KK31" s="0"/>
+      <c r="KL31" s="0"/>
+      <c r="KM31" s="0"/>
+      <c r="KN31" s="0"/>
+      <c r="KO31" s="0"/>
+      <c r="KP31" s="0"/>
+      <c r="KQ31" s="0"/>
+      <c r="KR31" s="0"/>
+      <c r="KS31" s="0"/>
+      <c r="KT31" s="0"/>
+      <c r="KU31" s="0"/>
+      <c r="KV31" s="0"/>
+      <c r="KW31" s="0"/>
+      <c r="KX31" s="0"/>
+      <c r="KY31" s="0"/>
+      <c r="KZ31" s="0"/>
+      <c r="LA31" s="0"/>
+      <c r="LB31" s="0"/>
+      <c r="LC31" s="0"/>
+      <c r="LD31" s="0"/>
+      <c r="LE31" s="0"/>
+      <c r="LF31" s="0"/>
+      <c r="LG31" s="0"/>
+      <c r="LH31" s="0"/>
+      <c r="LI31" s="0"/>
+      <c r="LJ31" s="0"/>
+      <c r="LK31" s="0"/>
+      <c r="LL31" s="0"/>
+      <c r="LM31" s="0"/>
+      <c r="LN31" s="0"/>
+      <c r="LO31" s="0"/>
+      <c r="LP31" s="0"/>
+      <c r="LQ31" s="0"/>
+      <c r="LR31" s="0"/>
+      <c r="LS31" s="0"/>
+      <c r="LT31" s="0"/>
+      <c r="LU31" s="0"/>
+      <c r="LV31" s="0"/>
+      <c r="LW31" s="0"/>
+      <c r="LX31" s="0"/>
+      <c r="LY31" s="0"/>
+      <c r="LZ31" s="0"/>
+      <c r="MA31" s="0"/>
+      <c r="MB31" s="0"/>
+      <c r="MC31" s="0"/>
+      <c r="MD31" s="0"/>
+      <c r="ME31" s="0"/>
+      <c r="MF31" s="0"/>
+      <c r="MG31" s="0"/>
+      <c r="MH31" s="0"/>
+      <c r="MI31" s="0"/>
+      <c r="MJ31" s="0"/>
+      <c r="MK31" s="0"/>
+      <c r="ML31" s="0"/>
+      <c r="MM31" s="0"/>
+      <c r="MN31" s="0"/>
+      <c r="MO31" s="0"/>
+      <c r="MP31" s="0"/>
+      <c r="MQ31" s="0"/>
+      <c r="MR31" s="0"/>
+      <c r="MS31" s="0"/>
+      <c r="MT31" s="0"/>
+      <c r="MU31" s="0"/>
+      <c r="MV31" s="0"/>
+      <c r="MW31" s="0"/>
+      <c r="MX31" s="0"/>
+      <c r="MY31" s="0"/>
+      <c r="MZ31" s="0"/>
+      <c r="NA31" s="0"/>
+      <c r="NB31" s="0"/>
+      <c r="NC31" s="0"/>
+      <c r="ND31" s="0"/>
+      <c r="NE31" s="0"/>
+      <c r="NF31" s="0"/>
+      <c r="NG31" s="0"/>
+      <c r="NH31" s="0"/>
+      <c r="NI31" s="0"/>
+      <c r="NJ31" s="0"/>
+      <c r="NK31" s="0"/>
+      <c r="NL31" s="0"/>
+      <c r="NM31" s="0"/>
+      <c r="NN31" s="0"/>
+      <c r="NO31" s="0"/>
+      <c r="NP31" s="0"/>
+      <c r="NQ31" s="0"/>
+      <c r="NR31" s="0"/>
+      <c r="NS31" s="0"/>
+      <c r="NT31" s="0"/>
+      <c r="NU31" s="0"/>
+      <c r="NV31" s="0"/>
+      <c r="NW31" s="0"/>
+      <c r="NX31" s="0"/>
+      <c r="NY31" s="0"/>
+      <c r="NZ31" s="0"/>
+      <c r="OA31" s="0"/>
+      <c r="OB31" s="0"/>
+      <c r="OC31" s="0"/>
+      <c r="OD31" s="0"/>
+      <c r="OE31" s="0"/>
+      <c r="OF31" s="0"/>
+      <c r="OG31" s="0"/>
+      <c r="OH31" s="0"/>
+      <c r="OI31" s="0"/>
+      <c r="OJ31" s="0"/>
+      <c r="OK31" s="0"/>
+      <c r="OL31" s="0"/>
+      <c r="OM31" s="0"/>
+      <c r="ON31" s="0"/>
+      <c r="OO31" s="0"/>
+      <c r="OP31" s="0"/>
+      <c r="OQ31" s="0"/>
+      <c r="OR31" s="0"/>
+      <c r="OS31" s="0"/>
+      <c r="OT31" s="0"/>
+      <c r="OU31" s="0"/>
+      <c r="OV31" s="0"/>
+      <c r="OW31" s="0"/>
+      <c r="OX31" s="0"/>
+      <c r="OY31" s="0"/>
+      <c r="OZ31" s="0"/>
+      <c r="PA31" s="0"/>
+      <c r="PB31" s="0"/>
+      <c r="PC31" s="0"/>
+      <c r="PD31" s="0"/>
+      <c r="PE31" s="0"/>
+      <c r="PF31" s="0"/>
+      <c r="PG31" s="0"/>
+      <c r="PH31" s="0"/>
+      <c r="PI31" s="0"/>
+      <c r="PJ31" s="0"/>
+      <c r="PK31" s="0"/>
+      <c r="PL31" s="0"/>
+      <c r="PM31" s="0"/>
+      <c r="PN31" s="0"/>
+      <c r="PO31" s="0"/>
+      <c r="PP31" s="0"/>
+      <c r="PQ31" s="0"/>
+      <c r="PR31" s="0"/>
+      <c r="PS31" s="0"/>
+      <c r="PT31" s="0"/>
+      <c r="PU31" s="0"/>
+      <c r="PV31" s="0"/>
+      <c r="PW31" s="0"/>
+      <c r="PX31" s="0"/>
+      <c r="PY31" s="0"/>
+      <c r="PZ31" s="0"/>
+      <c r="QA31" s="0"/>
+      <c r="QB31" s="0"/>
+      <c r="QC31" s="0"/>
+      <c r="QD31" s="0"/>
+      <c r="QE31" s="0"/>
+      <c r="QF31" s="0"/>
+      <c r="QG31" s="0"/>
+      <c r="QH31" s="0"/>
+      <c r="QI31" s="0"/>
+      <c r="QJ31" s="0"/>
+      <c r="QK31" s="0"/>
+      <c r="QL31" s="0"/>
+      <c r="QM31" s="0"/>
+      <c r="QN31" s="0"/>
+      <c r="QO31" s="0"/>
+      <c r="QP31" s="0"/>
+      <c r="QQ31" s="0"/>
+      <c r="QR31" s="0"/>
+      <c r="QS31" s="0"/>
+      <c r="QT31" s="0"/>
+      <c r="QU31" s="0"/>
+      <c r="QV31" s="0"/>
+      <c r="QW31" s="0"/>
+      <c r="QX31" s="0"/>
+      <c r="QY31" s="0"/>
+      <c r="QZ31" s="0"/>
+      <c r="RA31" s="0"/>
+      <c r="RB31" s="0"/>
+      <c r="RC31" s="0"/>
+      <c r="RD31" s="0"/>
+      <c r="RE31" s="0"/>
+      <c r="RF31" s="0"/>
+      <c r="RG31" s="0"/>
+      <c r="RH31" s="0"/>
+      <c r="RI31" s="0"/>
+      <c r="RJ31" s="0"/>
+      <c r="RK31" s="0"/>
+      <c r="RL31" s="0"/>
+      <c r="RM31" s="0"/>
+      <c r="RN31" s="0"/>
+      <c r="RO31" s="0"/>
+      <c r="RP31" s="0"/>
+      <c r="RQ31" s="0"/>
+      <c r="RR31" s="0"/>
+      <c r="RS31" s="0"/>
+      <c r="RT31" s="0"/>
+      <c r="RU31" s="0"/>
+      <c r="RV31" s="0"/>
+      <c r="RW31" s="0"/>
+      <c r="RX31" s="0"/>
+      <c r="RY31" s="0"/>
+      <c r="RZ31" s="0"/>
+      <c r="SA31" s="0"/>
+      <c r="SB31" s="0"/>
+      <c r="SC31" s="0"/>
+      <c r="SD31" s="0"/>
+      <c r="SE31" s="0"/>
+      <c r="SF31" s="0"/>
+      <c r="SG31" s="0"/>
+      <c r="SH31" s="0"/>
+      <c r="SI31" s="0"/>
+      <c r="SJ31" s="0"/>
+      <c r="SK31" s="0"/>
+      <c r="SL31" s="0"/>
+      <c r="SM31" s="0"/>
+      <c r="SN31" s="0"/>
+      <c r="SO31" s="0"/>
+      <c r="SP31" s="0"/>
+      <c r="SQ31" s="0"/>
+      <c r="SR31" s="0"/>
+      <c r="SS31" s="0"/>
+      <c r="ST31" s="0"/>
+      <c r="SU31" s="0"/>
+      <c r="SV31" s="0"/>
+      <c r="SW31" s="0"/>
+      <c r="SX31" s="0"/>
+      <c r="SY31" s="0"/>
+      <c r="SZ31" s="0"/>
+      <c r="TA31" s="0"/>
+      <c r="TB31" s="0"/>
+      <c r="TC31" s="0"/>
+      <c r="TD31" s="0"/>
+      <c r="TE31" s="0"/>
+      <c r="TF31" s="0"/>
+      <c r="TG31" s="0"/>
+      <c r="TH31" s="0"/>
+      <c r="TI31" s="0"/>
+      <c r="TJ31" s="0"/>
+      <c r="TK31" s="0"/>
+      <c r="TL31" s="0"/>
+      <c r="TM31" s="0"/>
+      <c r="TN31" s="0"/>
+      <c r="TO31" s="0"/>
+      <c r="TP31" s="0"/>
+      <c r="TQ31" s="0"/>
+      <c r="TR31" s="0"/>
+      <c r="TS31" s="0"/>
+      <c r="TT31" s="0"/>
+      <c r="TU31" s="0"/>
+      <c r="TV31" s="0"/>
+      <c r="TW31" s="0"/>
+      <c r="TX31" s="0"/>
+      <c r="TY31" s="0"/>
+      <c r="TZ31" s="0"/>
+      <c r="UA31" s="0"/>
+      <c r="UB31" s="0"/>
+      <c r="UC31" s="0"/>
+      <c r="UD31" s="0"/>
+      <c r="UE31" s="0"/>
+      <c r="UF31" s="0"/>
+      <c r="UG31" s="0"/>
+      <c r="UH31" s="0"/>
+      <c r="UI31" s="0"/>
+      <c r="UJ31" s="0"/>
+      <c r="UK31" s="0"/>
+      <c r="UL31" s="0"/>
+      <c r="UM31" s="0"/>
+      <c r="UN31" s="0"/>
+      <c r="UO31" s="0"/>
+      <c r="UP31" s="0"/>
+      <c r="UQ31" s="0"/>
+      <c r="UR31" s="0"/>
+      <c r="US31" s="0"/>
+      <c r="UT31" s="0"/>
+      <c r="UU31" s="0"/>
+      <c r="UV31" s="0"/>
+      <c r="UW31" s="0"/>
+      <c r="UX31" s="0"/>
+      <c r="UY31" s="0"/>
+      <c r="UZ31" s="0"/>
+      <c r="VA31" s="0"/>
+      <c r="VB31" s="0"/>
+      <c r="VC31" s="0"/>
+      <c r="VD31" s="0"/>
+      <c r="VE31" s="0"/>
+      <c r="VF31" s="0"/>
+      <c r="VG31" s="0"/>
+      <c r="VH31" s="0"/>
+      <c r="VI31" s="0"/>
+      <c r="VJ31" s="0"/>
+      <c r="VK31" s="0"/>
+      <c r="VL31" s="0"/>
+      <c r="VM31" s="0"/>
+      <c r="VN31" s="0"/>
+      <c r="VO31" s="0"/>
+      <c r="VP31" s="0"/>
+      <c r="VQ31" s="0"/>
+      <c r="VR31" s="0"/>
+      <c r="VS31" s="0"/>
+      <c r="VT31" s="0"/>
+      <c r="VU31" s="0"/>
+      <c r="VV31" s="0"/>
+      <c r="VW31" s="0"/>
+      <c r="VX31" s="0"/>
+      <c r="VY31" s="0"/>
+      <c r="VZ31" s="0"/>
+      <c r="WA31" s="0"/>
+      <c r="WB31" s="0"/>
+      <c r="WC31" s="0"/>
+      <c r="WD31" s="0"/>
+      <c r="WE31" s="0"/>
+      <c r="WF31" s="0"/>
+      <c r="WG31" s="0"/>
+      <c r="WH31" s="0"/>
+      <c r="WI31" s="0"/>
+      <c r="WJ31" s="0"/>
+      <c r="WK31" s="0"/>
+      <c r="WL31" s="0"/>
+      <c r="WM31" s="0"/>
+      <c r="WN31" s="0"/>
+      <c r="WO31" s="0"/>
+      <c r="WP31" s="0"/>
+      <c r="WQ31" s="0"/>
+      <c r="WR31" s="0"/>
+      <c r="WS31" s="0"/>
+      <c r="WT31" s="0"/>
+      <c r="WU31" s="0"/>
+      <c r="WV31" s="0"/>
+      <c r="WW31" s="0"/>
+      <c r="WX31" s="0"/>
+      <c r="WY31" s="0"/>
+      <c r="WZ31" s="0"/>
+      <c r="XA31" s="0"/>
+      <c r="XB31" s="0"/>
+      <c r="XC31" s="0"/>
+      <c r="XD31" s="0"/>
+      <c r="XE31" s="0"/>
+      <c r="XF31" s="0"/>
+      <c r="XG31" s="0"/>
+      <c r="XH31" s="0"/>
+      <c r="XI31" s="0"/>
+      <c r="XJ31" s="0"/>
+      <c r="XK31" s="0"/>
+      <c r="XL31" s="0"/>
+      <c r="XM31" s="0"/>
+      <c r="XN31" s="0"/>
+      <c r="XO31" s="0"/>
+      <c r="XP31" s="0"/>
+      <c r="XQ31" s="0"/>
+      <c r="XR31" s="0"/>
+      <c r="XS31" s="0"/>
+      <c r="XT31" s="0"/>
+      <c r="XU31" s="0"/>
+      <c r="XV31" s="0"/>
+      <c r="XW31" s="0"/>
+      <c r="XX31" s="0"/>
+      <c r="XY31" s="0"/>
+      <c r="XZ31" s="0"/>
+      <c r="YA31" s="0"/>
+      <c r="YB31" s="0"/>
+      <c r="YC31" s="0"/>
+      <c r="YD31" s="0"/>
+      <c r="YE31" s="0"/>
+      <c r="YF31" s="0"/>
+      <c r="YG31" s="0"/>
+      <c r="YH31" s="0"/>
+      <c r="YI31" s="0"/>
+      <c r="YJ31" s="0"/>
+      <c r="YK31" s="0"/>
+      <c r="YL31" s="0"/>
+      <c r="YM31" s="0"/>
+      <c r="YN31" s="0"/>
+      <c r="YO31" s="0"/>
+      <c r="YP31" s="0"/>
+      <c r="YQ31" s="0"/>
+      <c r="YR31" s="0"/>
+      <c r="YS31" s="0"/>
+      <c r="YT31" s="0"/>
+      <c r="YU31" s="0"/>
+      <c r="YV31" s="0"/>
+      <c r="YW31" s="0"/>
+      <c r="YX31" s="0"/>
+      <c r="YY31" s="0"/>
+      <c r="YZ31" s="0"/>
+      <c r="ZA31" s="0"/>
+      <c r="ZB31" s="0"/>
+      <c r="ZC31" s="0"/>
+      <c r="ZD31" s="0"/>
+      <c r="ZE31" s="0"/>
+      <c r="ZF31" s="0"/>
+      <c r="ZG31" s="0"/>
+      <c r="ZH31" s="0"/>
+      <c r="ZI31" s="0"/>
+      <c r="ZJ31" s="0"/>
+      <c r="ZK31" s="0"/>
+      <c r="ZL31" s="0"/>
+      <c r="ZM31" s="0"/>
+      <c r="ZN31" s="0"/>
+      <c r="ZO31" s="0"/>
+      <c r="ZP31" s="0"/>
+      <c r="ZQ31" s="0"/>
+      <c r="ZR31" s="0"/>
+      <c r="ZS31" s="0"/>
+      <c r="ZT31" s="0"/>
+      <c r="ZU31" s="0"/>
+      <c r="ZV31" s="0"/>
+      <c r="ZW31" s="0"/>
+      <c r="ZX31" s="0"/>
+      <c r="ZY31" s="0"/>
+      <c r="ZZ31" s="0"/>
+      <c r="AAA31" s="0"/>
+      <c r="AAB31" s="0"/>
+      <c r="AAC31" s="0"/>
+      <c r="AAD31" s="0"/>
+      <c r="AAE31" s="0"/>
+      <c r="AAF31" s="0"/>
+      <c r="AAG31" s="0"/>
+      <c r="AAH31" s="0"/>
+      <c r="AAI31" s="0"/>
+      <c r="AAJ31" s="0"/>
+      <c r="AAK31" s="0"/>
+      <c r="AAL31" s="0"/>
+      <c r="AAM31" s="0"/>
+      <c r="AAN31" s="0"/>
+      <c r="AAO31" s="0"/>
+      <c r="AAP31" s="0"/>
+      <c r="AAQ31" s="0"/>
+      <c r="AAR31" s="0"/>
+      <c r="AAS31" s="0"/>
+      <c r="AAT31" s="0"/>
+      <c r="AAU31" s="0"/>
+      <c r="AAV31" s="0"/>
+      <c r="AAW31" s="0"/>
+      <c r="AAX31" s="0"/>
+      <c r="AAY31" s="0"/>
+      <c r="AAZ31" s="0"/>
+      <c r="ABA31" s="0"/>
+      <c r="ABB31" s="0"/>
+      <c r="ABC31" s="0"/>
+      <c r="ABD31" s="0"/>
+      <c r="ABE31" s="0"/>
+      <c r="ABF31" s="0"/>
+      <c r="ABG31" s="0"/>
+      <c r="ABH31" s="0"/>
+      <c r="ABI31" s="0"/>
+      <c r="ABJ31" s="0"/>
+      <c r="ABK31" s="0"/>
+      <c r="ABL31" s="0"/>
+      <c r="ABM31" s="0"/>
+      <c r="ABN31" s="0"/>
+      <c r="ABO31" s="0"/>
+      <c r="ABP31" s="0"/>
+      <c r="ABQ31" s="0"/>
+      <c r="ABR31" s="0"/>
+      <c r="ABS31" s="0"/>
+      <c r="ABT31" s="0"/>
+      <c r="ABU31" s="0"/>
+      <c r="ABV31" s="0"/>
+      <c r="ABW31" s="0"/>
+      <c r="ABX31" s="0"/>
+      <c r="ABY31" s="0"/>
+      <c r="ABZ31" s="0"/>
+      <c r="ACA31" s="0"/>
+      <c r="ACB31" s="0"/>
+      <c r="ACC31" s="0"/>
+      <c r="ACD31" s="0"/>
+      <c r="ACE31" s="0"/>
+      <c r="ACF31" s="0"/>
+      <c r="ACG31" s="0"/>
+      <c r="ACH31" s="0"/>
+      <c r="ACI31" s="0"/>
+      <c r="ACJ31" s="0"/>
+      <c r="ACK31" s="0"/>
+      <c r="ACL31" s="0"/>
+      <c r="ACM31" s="0"/>
+      <c r="ACN31" s="0"/>
+      <c r="ACO31" s="0"/>
+      <c r="ACP31" s="0"/>
+      <c r="ACQ31" s="0"/>
+      <c r="ACR31" s="0"/>
+      <c r="ACS31" s="0"/>
+      <c r="ACT31" s="0"/>
+      <c r="ACU31" s="0"/>
+      <c r="ACV31" s="0"/>
+      <c r="ACW31" s="0"/>
+      <c r="ACX31" s="0"/>
+      <c r="ACY31" s="0"/>
+      <c r="ACZ31" s="0"/>
+      <c r="ADA31" s="0"/>
+      <c r="ADB31" s="0"/>
+      <c r="ADC31" s="0"/>
+      <c r="ADD31" s="0"/>
+      <c r="ADE31" s="0"/>
+      <c r="ADF31" s="0"/>
+      <c r="ADG31" s="0"/>
+      <c r="ADH31" s="0"/>
+      <c r="ADI31" s="0"/>
+      <c r="ADJ31" s="0"/>
+      <c r="ADK31" s="0"/>
+      <c r="ADL31" s="0"/>
+      <c r="ADM31" s="0"/>
+      <c r="ADN31" s="0"/>
+      <c r="ADO31" s="0"/>
+      <c r="ADP31" s="0"/>
+      <c r="ADQ31" s="0"/>
+      <c r="ADR31" s="0"/>
+      <c r="ADS31" s="0"/>
+      <c r="ADT31" s="0"/>
+      <c r="ADU31" s="0"/>
+      <c r="ADV31" s="0"/>
+      <c r="ADW31" s="0"/>
+      <c r="ADX31" s="0"/>
+      <c r="ADY31" s="0"/>
+      <c r="ADZ31" s="0"/>
+      <c r="AEA31" s="0"/>
+      <c r="AEB31" s="0"/>
+      <c r="AEC31" s="0"/>
+      <c r="AED31" s="0"/>
+      <c r="AEE31" s="0"/>
+      <c r="AEF31" s="0"/>
+      <c r="AEG31" s="0"/>
+      <c r="AEH31" s="0"/>
+      <c r="AEI31" s="0"/>
+      <c r="AEJ31" s="0"/>
+      <c r="AEK31" s="0"/>
+      <c r="AEL31" s="0"/>
+      <c r="AEM31" s="0"/>
+      <c r="AEN31" s="0"/>
+      <c r="AEO31" s="0"/>
+      <c r="AEP31" s="0"/>
+      <c r="AEQ31" s="0"/>
+      <c r="AER31" s="0"/>
+      <c r="AES31" s="0"/>
+      <c r="AET31" s="0"/>
+      <c r="AEU31" s="0"/>
+      <c r="AEV31" s="0"/>
+      <c r="AEW31" s="0"/>
+      <c r="AEX31" s="0"/>
+      <c r="AEY31" s="0"/>
+      <c r="AEZ31" s="0"/>
+      <c r="AFA31" s="0"/>
+      <c r="AFB31" s="0"/>
+      <c r="AFC31" s="0"/>
+      <c r="AFD31" s="0"/>
+      <c r="AFE31" s="0"/>
+      <c r="AFF31" s="0"/>
+      <c r="AFG31" s="0"/>
+      <c r="AFH31" s="0"/>
+      <c r="AFI31" s="0"/>
+      <c r="AFJ31" s="0"/>
+      <c r="AFK31" s="0"/>
+      <c r="AFL31" s="0"/>
+      <c r="AFM31" s="0"/>
+      <c r="AFN31" s="0"/>
+      <c r="AFO31" s="0"/>
+      <c r="AFP31" s="0"/>
+      <c r="AFQ31" s="0"/>
+      <c r="AFR31" s="0"/>
+      <c r="AFS31" s="0"/>
+      <c r="AFT31" s="0"/>
+      <c r="AFU31" s="0"/>
+      <c r="AFV31" s="0"/>
+      <c r="AFW31" s="0"/>
+      <c r="AFX31" s="0"/>
+      <c r="AFY31" s="0"/>
+      <c r="AFZ31" s="0"/>
+      <c r="AGA31" s="0"/>
+      <c r="AGB31" s="0"/>
+      <c r="AGC31" s="0"/>
+      <c r="AGD31" s="0"/>
+      <c r="AGE31" s="0"/>
+      <c r="AGF31" s="0"/>
+      <c r="AGG31" s="0"/>
+      <c r="AGH31" s="0"/>
+      <c r="AGI31" s="0"/>
+      <c r="AGJ31" s="0"/>
+      <c r="AGK31" s="0"/>
+      <c r="AGL31" s="0"/>
+      <c r="AGM31" s="0"/>
+      <c r="AGN31" s="0"/>
+      <c r="AGO31" s="0"/>
+      <c r="AGP31" s="0"/>
+      <c r="AGQ31" s="0"/>
+      <c r="AGR31" s="0"/>
+      <c r="AGS31" s="0"/>
+      <c r="AGT31" s="0"/>
+      <c r="AGU31" s="0"/>
+      <c r="AGV31" s="0"/>
+      <c r="AGW31" s="0"/>
+      <c r="AGX31" s="0"/>
+      <c r="AGY31" s="0"/>
+      <c r="AGZ31" s="0"/>
+      <c r="AHA31" s="0"/>
+      <c r="AHB31" s="0"/>
+      <c r="AHC31" s="0"/>
+      <c r="AHD31" s="0"/>
+      <c r="AHE31" s="0"/>
+      <c r="AHF31" s="0"/>
+      <c r="AHG31" s="0"/>
+      <c r="AHH31" s="0"/>
+      <c r="AHI31" s="0"/>
+      <c r="AHJ31" s="0"/>
+      <c r="AHK31" s="0"/>
+      <c r="AHL31" s="0"/>
+      <c r="AHM31" s="0"/>
+      <c r="AHN31" s="0"/>
+      <c r="AHO31" s="0"/>
+      <c r="AHP31" s="0"/>
+      <c r="AHQ31" s="0"/>
+      <c r="AHR31" s="0"/>
+      <c r="AHS31" s="0"/>
+      <c r="AHT31" s="0"/>
+      <c r="AHU31" s="0"/>
+      <c r="AHV31" s="0"/>
+      <c r="AHW31" s="0"/>
+      <c r="AHX31" s="0"/>
+      <c r="AHY31" s="0"/>
+      <c r="AHZ31" s="0"/>
+      <c r="AIA31" s="0"/>
+      <c r="AIB31" s="0"/>
+      <c r="AIC31" s="0"/>
+      <c r="AID31" s="0"/>
+      <c r="AIE31" s="0"/>
+      <c r="AIF31" s="0"/>
+      <c r="AIG31" s="0"/>
+      <c r="AIH31" s="0"/>
+      <c r="AII31" s="0"/>
+      <c r="AIJ31" s="0"/>
+      <c r="AIK31" s="0"/>
+      <c r="AIL31" s="0"/>
+      <c r="AIM31" s="0"/>
+      <c r="AIN31" s="0"/>
+      <c r="AIO31" s="0"/>
+      <c r="AIP31" s="0"/>
+      <c r="AIQ31" s="0"/>
+      <c r="AIR31" s="0"/>
+      <c r="AIS31" s="0"/>
+      <c r="AIT31" s="0"/>
+      <c r="AIU31" s="0"/>
+      <c r="AIV31" s="0"/>
+      <c r="AIW31" s="0"/>
+      <c r="AIX31" s="0"/>
+      <c r="AIY31" s="0"/>
+      <c r="AIZ31" s="0"/>
+      <c r="AJA31" s="0"/>
+      <c r="AJB31" s="0"/>
+      <c r="AJC31" s="0"/>
+      <c r="AJD31" s="0"/>
+      <c r="AJE31" s="0"/>
+      <c r="AJF31" s="0"/>
+      <c r="AJG31" s="0"/>
+      <c r="AJH31" s="0"/>
+      <c r="AJI31" s="0"/>
+      <c r="AJJ31" s="0"/>
+      <c r="AJK31" s="0"/>
+      <c r="AJL31" s="0"/>
+      <c r="AJM31" s="0"/>
+      <c r="AJN31" s="0"/>
+      <c r="AJO31" s="0"/>
+      <c r="AJP31" s="0"/>
+      <c r="AJQ31" s="0"/>
+      <c r="AJR31" s="0"/>
+      <c r="AJS31" s="0"/>
+      <c r="AJT31" s="0"/>
+      <c r="AJU31" s="0"/>
+      <c r="AJV31" s="0"/>
+      <c r="AJW31" s="0"/>
+      <c r="AJX31" s="0"/>
+      <c r="AJY31" s="0"/>
+      <c r="AJZ31" s="0"/>
+      <c r="AKA31" s="0"/>
+      <c r="AKB31" s="0"/>
+      <c r="AKC31" s="0"/>
+      <c r="AKD31" s="0"/>
+      <c r="AKE31" s="0"/>
+      <c r="AKF31" s="0"/>
+      <c r="AKG31" s="0"/>
+      <c r="AKH31" s="0"/>
+      <c r="AKI31" s="0"/>
+      <c r="AKJ31" s="0"/>
+      <c r="AKK31" s="0"/>
+      <c r="AKL31" s="0"/>
+      <c r="AKM31" s="0"/>
+      <c r="AKN31" s="0"/>
+      <c r="AKO31" s="0"/>
+      <c r="AKP31" s="0"/>
+      <c r="AKQ31" s="0"/>
+      <c r="AKR31" s="0"/>
+      <c r="AKS31" s="0"/>
+      <c r="AKT31" s="0"/>
+      <c r="AKU31" s="0"/>
+      <c r="AKV31" s="0"/>
+      <c r="AKW31" s="0"/>
+      <c r="AKX31" s="0"/>
+      <c r="AKY31" s="0"/>
+      <c r="AKZ31" s="0"/>
+      <c r="ALA31" s="0"/>
+      <c r="ALB31" s="0"/>
+      <c r="ALC31" s="0"/>
+      <c r="ALD31" s="0"/>
+      <c r="ALE31" s="0"/>
+      <c r="ALF31" s="0"/>
+      <c r="ALG31" s="0"/>
+      <c r="ALH31" s="0"/>
+      <c r="ALI31" s="0"/>
+      <c r="ALJ31" s="0"/>
+      <c r="ALK31" s="0"/>
+      <c r="ALL31" s="0"/>
+      <c r="ALM31" s="0"/>
+      <c r="ALN31" s="0"/>
+      <c r="ALO31" s="0"/>
+      <c r="ALP31" s="0"/>
+      <c r="ALQ31" s="0"/>
+      <c r="ALR31" s="0"/>
+      <c r="ALS31" s="0"/>
+      <c r="ALT31" s="0"/>
+      <c r="ALU31" s="0"/>
+      <c r="ALV31" s="0"/>
+      <c r="ALW31" s="0"/>
+      <c r="ALX31" s="0"/>
+      <c r="ALY31" s="0"/>
+      <c r="ALZ31" s="0"/>
+      <c r="AMA31" s="0"/>
+      <c r="AMB31" s="0"/>
+      <c r="AMC31" s="0"/>
+      <c r="AMD31" s="0"/>
+      <c r="AME31" s="0"/>
+      <c r="AMF31" s="0"/>
+      <c r="AMG31" s="0"/>
+      <c r="AMH31" s="0"/>
+      <c r="AMI31" s="0"/>
+      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="21"/>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
@@ -25468,15 +25449,15 @@
       <c r="A33" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
+      <c r="J33" s="24"/>
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
       <c r="M33" s="21"/>
@@ -26496,8 +26477,8 @@
       <c r="A34" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
@@ -26506,7 +26487,7 @@
       <c r="I34" s="21"/>
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
+      <c r="L34" s="24"/>
       <c r="M34" s="21"/>
       <c r="N34" s="0"/>
       <c r="O34" s="0"/>
@@ -27520,2148 +27501,94 @@
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21" t="s">
+    <row r="35" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="0"/>
-      <c r="O35" s="0"/>
-      <c r="P35" s="0"/>
-      <c r="Q35" s="0"/>
-      <c r="R35" s="0"/>
-      <c r="S35" s="0"/>
-      <c r="T35" s="0"/>
-      <c r="U35" s="0"/>
-      <c r="V35" s="0"/>
-      <c r="W35" s="0"/>
-      <c r="X35" s="0"/>
-      <c r="Y35" s="0"/>
-      <c r="Z35" s="0"/>
-      <c r="AA35" s="0"/>
-      <c r="AB35" s="0"/>
-      <c r="AC35" s="0"/>
-      <c r="AD35" s="0"/>
-      <c r="AE35" s="0"/>
-      <c r="AF35" s="0"/>
-      <c r="AG35" s="0"/>
-      <c r="AH35" s="0"/>
-      <c r="AI35" s="0"/>
-      <c r="AJ35" s="0"/>
-      <c r="AK35" s="0"/>
-      <c r="AL35" s="0"/>
-      <c r="AM35" s="0"/>
-      <c r="AN35" s="0"/>
-      <c r="AO35" s="0"/>
-      <c r="AP35" s="0"/>
-      <c r="AQ35" s="0"/>
-      <c r="AR35" s="0"/>
-      <c r="AS35" s="0"/>
-      <c r="AT35" s="0"/>
-      <c r="AU35" s="0"/>
-      <c r="AV35" s="0"/>
-      <c r="AW35" s="0"/>
-      <c r="AX35" s="0"/>
-      <c r="AY35" s="0"/>
-      <c r="AZ35" s="0"/>
-      <c r="BA35" s="0"/>
-      <c r="BB35" s="0"/>
-      <c r="BC35" s="0"/>
-      <c r="BD35" s="0"/>
-      <c r="BE35" s="0"/>
-      <c r="BF35" s="0"/>
-      <c r="BG35" s="0"/>
-      <c r="BH35" s="0"/>
-      <c r="BI35" s="0"/>
-      <c r="BJ35" s="0"/>
-      <c r="BK35" s="0"/>
-      <c r="BL35" s="0"/>
-      <c r="BM35" s="0"/>
-      <c r="BN35" s="0"/>
-      <c r="BO35" s="0"/>
-      <c r="BP35" s="0"/>
-      <c r="BQ35" s="0"/>
-      <c r="BR35" s="0"/>
-      <c r="BS35" s="0"/>
-      <c r="BT35" s="0"/>
-      <c r="BU35" s="0"/>
-      <c r="BV35" s="0"/>
-      <c r="BW35" s="0"/>
-      <c r="BX35" s="0"/>
-      <c r="BY35" s="0"/>
-      <c r="BZ35" s="0"/>
-      <c r="CA35" s="0"/>
-      <c r="CB35" s="0"/>
-      <c r="CC35" s="0"/>
-      <c r="CD35" s="0"/>
-      <c r="CE35" s="0"/>
-      <c r="CF35" s="0"/>
-      <c r="CG35" s="0"/>
-      <c r="CH35" s="0"/>
-      <c r="CI35" s="0"/>
-      <c r="CJ35" s="0"/>
-      <c r="CK35" s="0"/>
-      <c r="CL35" s="0"/>
-      <c r="CM35" s="0"/>
-      <c r="CN35" s="0"/>
-      <c r="CO35" s="0"/>
-      <c r="CP35" s="0"/>
-      <c r="CQ35" s="0"/>
-      <c r="CR35" s="0"/>
-      <c r="CS35" s="0"/>
-      <c r="CT35" s="0"/>
-      <c r="CU35" s="0"/>
-      <c r="CV35" s="0"/>
-      <c r="CW35" s="0"/>
-      <c r="CX35" s="0"/>
-      <c r="CY35" s="0"/>
-      <c r="CZ35" s="0"/>
-      <c r="DA35" s="0"/>
-      <c r="DB35" s="0"/>
-      <c r="DC35" s="0"/>
-      <c r="DD35" s="0"/>
-      <c r="DE35" s="0"/>
-      <c r="DF35" s="0"/>
-      <c r="DG35" s="0"/>
-      <c r="DH35" s="0"/>
-      <c r="DI35" s="0"/>
-      <c r="DJ35" s="0"/>
-      <c r="DK35" s="0"/>
-      <c r="DL35" s="0"/>
-      <c r="DM35" s="0"/>
-      <c r="DN35" s="0"/>
-      <c r="DO35" s="0"/>
-      <c r="DP35" s="0"/>
-      <c r="DQ35" s="0"/>
-      <c r="DR35" s="0"/>
-      <c r="DS35" s="0"/>
-      <c r="DT35" s="0"/>
-      <c r="DU35" s="0"/>
-      <c r="DV35" s="0"/>
-      <c r="DW35" s="0"/>
-      <c r="DX35" s="0"/>
-      <c r="DY35" s="0"/>
-      <c r="DZ35" s="0"/>
-      <c r="EA35" s="0"/>
-      <c r="EB35" s="0"/>
-      <c r="EC35" s="0"/>
-      <c r="ED35" s="0"/>
-      <c r="EE35" s="0"/>
-      <c r="EF35" s="0"/>
-      <c r="EG35" s="0"/>
-      <c r="EH35" s="0"/>
-      <c r="EI35" s="0"/>
-      <c r="EJ35" s="0"/>
-      <c r="EK35" s="0"/>
-      <c r="EL35" s="0"/>
-      <c r="EM35" s="0"/>
-      <c r="EN35" s="0"/>
-      <c r="EO35" s="0"/>
-      <c r="EP35" s="0"/>
-      <c r="EQ35" s="0"/>
-      <c r="ER35" s="0"/>
-      <c r="ES35" s="0"/>
-      <c r="ET35" s="0"/>
-      <c r="EU35" s="0"/>
-      <c r="EV35" s="0"/>
-      <c r="EW35" s="0"/>
-      <c r="EX35" s="0"/>
-      <c r="EY35" s="0"/>
-      <c r="EZ35" s="0"/>
-      <c r="FA35" s="0"/>
-      <c r="FB35" s="0"/>
-      <c r="FC35" s="0"/>
-      <c r="FD35" s="0"/>
-      <c r="FE35" s="0"/>
-      <c r="FF35" s="0"/>
-      <c r="FG35" s="0"/>
-      <c r="FH35" s="0"/>
-      <c r="FI35" s="0"/>
-      <c r="FJ35" s="0"/>
-      <c r="FK35" s="0"/>
-      <c r="FL35" s="0"/>
-      <c r="FM35" s="0"/>
-      <c r="FN35" s="0"/>
-      <c r="FO35" s="0"/>
-      <c r="FP35" s="0"/>
-      <c r="FQ35" s="0"/>
-      <c r="FR35" s="0"/>
-      <c r="FS35" s="0"/>
-      <c r="FT35" s="0"/>
-      <c r="FU35" s="0"/>
-      <c r="FV35" s="0"/>
-      <c r="FW35" s="0"/>
-      <c r="FX35" s="0"/>
-      <c r="FY35" s="0"/>
-      <c r="FZ35" s="0"/>
-      <c r="GA35" s="0"/>
-      <c r="GB35" s="0"/>
-      <c r="GC35" s="0"/>
-      <c r="GD35" s="0"/>
-      <c r="GE35" s="0"/>
-      <c r="GF35" s="0"/>
-      <c r="GG35" s="0"/>
-      <c r="GH35" s="0"/>
-      <c r="GI35" s="0"/>
-      <c r="GJ35" s="0"/>
-      <c r="GK35" s="0"/>
-      <c r="GL35" s="0"/>
-      <c r="GM35" s="0"/>
-      <c r="GN35" s="0"/>
-      <c r="GO35" s="0"/>
-      <c r="GP35" s="0"/>
-      <c r="GQ35" s="0"/>
-      <c r="GR35" s="0"/>
-      <c r="GS35" s="0"/>
-      <c r="GT35" s="0"/>
-      <c r="GU35" s="0"/>
-      <c r="GV35" s="0"/>
-      <c r="GW35" s="0"/>
-      <c r="GX35" s="0"/>
-      <c r="GY35" s="0"/>
-      <c r="GZ35" s="0"/>
-      <c r="HA35" s="0"/>
-      <c r="HB35" s="0"/>
-      <c r="HC35" s="0"/>
-      <c r="HD35" s="0"/>
-      <c r="HE35" s="0"/>
-      <c r="HF35" s="0"/>
-      <c r="HG35" s="0"/>
-      <c r="HH35" s="0"/>
-      <c r="HI35" s="0"/>
-      <c r="HJ35" s="0"/>
-      <c r="HK35" s="0"/>
-      <c r="HL35" s="0"/>
-      <c r="HM35" s="0"/>
-      <c r="HN35" s="0"/>
-      <c r="HO35" s="0"/>
-      <c r="HP35" s="0"/>
-      <c r="HQ35" s="0"/>
-      <c r="HR35" s="0"/>
-      <c r="HS35" s="0"/>
-      <c r="HT35" s="0"/>
-      <c r="HU35" s="0"/>
-      <c r="HV35" s="0"/>
-      <c r="HW35" s="0"/>
-      <c r="HX35" s="0"/>
-      <c r="HY35" s="0"/>
-      <c r="HZ35" s="0"/>
-      <c r="IA35" s="0"/>
-      <c r="IB35" s="0"/>
-      <c r="IC35" s="0"/>
-      <c r="ID35" s="0"/>
-      <c r="IE35" s="0"/>
-      <c r="IF35" s="0"/>
-      <c r="IG35" s="0"/>
-      <c r="IH35" s="0"/>
-      <c r="II35" s="0"/>
-      <c r="IJ35" s="0"/>
-      <c r="IK35" s="0"/>
-      <c r="IL35" s="0"/>
-      <c r="IM35" s="0"/>
-      <c r="IN35" s="0"/>
-      <c r="IO35" s="0"/>
-      <c r="IP35" s="0"/>
-      <c r="IQ35" s="0"/>
-      <c r="IR35" s="0"/>
-      <c r="IS35" s="0"/>
-      <c r="IT35" s="0"/>
-      <c r="IU35" s="0"/>
-      <c r="IV35" s="0"/>
-      <c r="IW35" s="0"/>
-      <c r="IX35" s="0"/>
-      <c r="IY35" s="0"/>
-      <c r="IZ35" s="0"/>
-      <c r="JA35" s="0"/>
-      <c r="JB35" s="0"/>
-      <c r="JC35" s="0"/>
-      <c r="JD35" s="0"/>
-      <c r="JE35" s="0"/>
-      <c r="JF35" s="0"/>
-      <c r="JG35" s="0"/>
-      <c r="JH35" s="0"/>
-      <c r="JI35" s="0"/>
-      <c r="JJ35" s="0"/>
-      <c r="JK35" s="0"/>
-      <c r="JL35" s="0"/>
-      <c r="JM35" s="0"/>
-      <c r="JN35" s="0"/>
-      <c r="JO35" s="0"/>
-      <c r="JP35" s="0"/>
-      <c r="JQ35" s="0"/>
-      <c r="JR35" s="0"/>
-      <c r="JS35" s="0"/>
-      <c r="JT35" s="0"/>
-      <c r="JU35" s="0"/>
-      <c r="JV35" s="0"/>
-      <c r="JW35" s="0"/>
-      <c r="JX35" s="0"/>
-      <c r="JY35" s="0"/>
-      <c r="JZ35" s="0"/>
-      <c r="KA35" s="0"/>
-      <c r="KB35" s="0"/>
-      <c r="KC35" s="0"/>
-      <c r="KD35" s="0"/>
-      <c r="KE35" s="0"/>
-      <c r="KF35" s="0"/>
-      <c r="KG35" s="0"/>
-      <c r="KH35" s="0"/>
-      <c r="KI35" s="0"/>
-      <c r="KJ35" s="0"/>
-      <c r="KK35" s="0"/>
-      <c r="KL35" s="0"/>
-      <c r="KM35" s="0"/>
-      <c r="KN35" s="0"/>
-      <c r="KO35" s="0"/>
-      <c r="KP35" s="0"/>
-      <c r="KQ35" s="0"/>
-      <c r="KR35" s="0"/>
-      <c r="KS35" s="0"/>
-      <c r="KT35" s="0"/>
-      <c r="KU35" s="0"/>
-      <c r="KV35" s="0"/>
-      <c r="KW35" s="0"/>
-      <c r="KX35" s="0"/>
-      <c r="KY35" s="0"/>
-      <c r="KZ35" s="0"/>
-      <c r="LA35" s="0"/>
-      <c r="LB35" s="0"/>
-      <c r="LC35" s="0"/>
-      <c r="LD35" s="0"/>
-      <c r="LE35" s="0"/>
-      <c r="LF35" s="0"/>
-      <c r="LG35" s="0"/>
-      <c r="LH35" s="0"/>
-      <c r="LI35" s="0"/>
-      <c r="LJ35" s="0"/>
-      <c r="LK35" s="0"/>
-      <c r="LL35" s="0"/>
-      <c r="LM35" s="0"/>
-      <c r="LN35" s="0"/>
-      <c r="LO35" s="0"/>
-      <c r="LP35" s="0"/>
-      <c r="LQ35" s="0"/>
-      <c r="LR35" s="0"/>
-      <c r="LS35" s="0"/>
-      <c r="LT35" s="0"/>
-      <c r="LU35" s="0"/>
-      <c r="LV35" s="0"/>
-      <c r="LW35" s="0"/>
-      <c r="LX35" s="0"/>
-      <c r="LY35" s="0"/>
-      <c r="LZ35" s="0"/>
-      <c r="MA35" s="0"/>
-      <c r="MB35" s="0"/>
-      <c r="MC35" s="0"/>
-      <c r="MD35" s="0"/>
-      <c r="ME35" s="0"/>
-      <c r="MF35" s="0"/>
-      <c r="MG35" s="0"/>
-      <c r="MH35" s="0"/>
-      <c r="MI35" s="0"/>
-      <c r="MJ35" s="0"/>
-      <c r="MK35" s="0"/>
-      <c r="ML35" s="0"/>
-      <c r="MM35" s="0"/>
-      <c r="MN35" s="0"/>
-      <c r="MO35" s="0"/>
-      <c r="MP35" s="0"/>
-      <c r="MQ35" s="0"/>
-      <c r="MR35" s="0"/>
-      <c r="MS35" s="0"/>
-      <c r="MT35" s="0"/>
-      <c r="MU35" s="0"/>
-      <c r="MV35" s="0"/>
-      <c r="MW35" s="0"/>
-      <c r="MX35" s="0"/>
-      <c r="MY35" s="0"/>
-      <c r="MZ35" s="0"/>
-      <c r="NA35" s="0"/>
-      <c r="NB35" s="0"/>
-      <c r="NC35" s="0"/>
-      <c r="ND35" s="0"/>
-      <c r="NE35" s="0"/>
-      <c r="NF35" s="0"/>
-      <c r="NG35" s="0"/>
-      <c r="NH35" s="0"/>
-      <c r="NI35" s="0"/>
-      <c r="NJ35" s="0"/>
-      <c r="NK35" s="0"/>
-      <c r="NL35" s="0"/>
-      <c r="NM35" s="0"/>
-      <c r="NN35" s="0"/>
-      <c r="NO35" s="0"/>
-      <c r="NP35" s="0"/>
-      <c r="NQ35" s="0"/>
-      <c r="NR35" s="0"/>
-      <c r="NS35" s="0"/>
-      <c r="NT35" s="0"/>
-      <c r="NU35" s="0"/>
-      <c r="NV35" s="0"/>
-      <c r="NW35" s="0"/>
-      <c r="NX35" s="0"/>
-      <c r="NY35" s="0"/>
-      <c r="NZ35" s="0"/>
-      <c r="OA35" s="0"/>
-      <c r="OB35" s="0"/>
-      <c r="OC35" s="0"/>
-      <c r="OD35" s="0"/>
-      <c r="OE35" s="0"/>
-      <c r="OF35" s="0"/>
-      <c r="OG35" s="0"/>
-      <c r="OH35" s="0"/>
-      <c r="OI35" s="0"/>
-      <c r="OJ35" s="0"/>
-      <c r="OK35" s="0"/>
-      <c r="OL35" s="0"/>
-      <c r="OM35" s="0"/>
-      <c r="ON35" s="0"/>
-      <c r="OO35" s="0"/>
-      <c r="OP35" s="0"/>
-      <c r="OQ35" s="0"/>
-      <c r="OR35" s="0"/>
-      <c r="OS35" s="0"/>
-      <c r="OT35" s="0"/>
-      <c r="OU35" s="0"/>
-      <c r="OV35" s="0"/>
-      <c r="OW35" s="0"/>
-      <c r="OX35" s="0"/>
-      <c r="OY35" s="0"/>
-      <c r="OZ35" s="0"/>
-      <c r="PA35" s="0"/>
-      <c r="PB35" s="0"/>
-      <c r="PC35" s="0"/>
-      <c r="PD35" s="0"/>
-      <c r="PE35" s="0"/>
-      <c r="PF35" s="0"/>
-      <c r="PG35" s="0"/>
-      <c r="PH35" s="0"/>
-      <c r="PI35" s="0"/>
-      <c r="PJ35" s="0"/>
-      <c r="PK35" s="0"/>
-      <c r="PL35" s="0"/>
-      <c r="PM35" s="0"/>
-      <c r="PN35" s="0"/>
-      <c r="PO35" s="0"/>
-      <c r="PP35" s="0"/>
-      <c r="PQ35" s="0"/>
-      <c r="PR35" s="0"/>
-      <c r="PS35" s="0"/>
-      <c r="PT35" s="0"/>
-      <c r="PU35" s="0"/>
-      <c r="PV35" s="0"/>
-      <c r="PW35" s="0"/>
-      <c r="PX35" s="0"/>
-      <c r="PY35" s="0"/>
-      <c r="PZ35" s="0"/>
-      <c r="QA35" s="0"/>
-      <c r="QB35" s="0"/>
-      <c r="QC35" s="0"/>
-      <c r="QD35" s="0"/>
-      <c r="QE35" s="0"/>
-      <c r="QF35" s="0"/>
-      <c r="QG35" s="0"/>
-      <c r="QH35" s="0"/>
-      <c r="QI35" s="0"/>
-      <c r="QJ35" s="0"/>
-      <c r="QK35" s="0"/>
-      <c r="QL35" s="0"/>
-      <c r="QM35" s="0"/>
-      <c r="QN35" s="0"/>
-      <c r="QO35" s="0"/>
-      <c r="QP35" s="0"/>
-      <c r="QQ35" s="0"/>
-      <c r="QR35" s="0"/>
-      <c r="QS35" s="0"/>
-      <c r="QT35" s="0"/>
-      <c r="QU35" s="0"/>
-      <c r="QV35" s="0"/>
-      <c r="QW35" s="0"/>
-      <c r="QX35" s="0"/>
-      <c r="QY35" s="0"/>
-      <c r="QZ35" s="0"/>
-      <c r="RA35" s="0"/>
-      <c r="RB35" s="0"/>
-      <c r="RC35" s="0"/>
-      <c r="RD35" s="0"/>
-      <c r="RE35" s="0"/>
-      <c r="RF35" s="0"/>
-      <c r="RG35" s="0"/>
-      <c r="RH35" s="0"/>
-      <c r="RI35" s="0"/>
-      <c r="RJ35" s="0"/>
-      <c r="RK35" s="0"/>
-      <c r="RL35" s="0"/>
-      <c r="RM35" s="0"/>
-      <c r="RN35" s="0"/>
-      <c r="RO35" s="0"/>
-      <c r="RP35" s="0"/>
-      <c r="RQ35" s="0"/>
-      <c r="RR35" s="0"/>
-      <c r="RS35" s="0"/>
-      <c r="RT35" s="0"/>
-      <c r="RU35" s="0"/>
-      <c r="RV35" s="0"/>
-      <c r="RW35" s="0"/>
-      <c r="RX35" s="0"/>
-      <c r="RY35" s="0"/>
-      <c r="RZ35" s="0"/>
-      <c r="SA35" s="0"/>
-      <c r="SB35" s="0"/>
-      <c r="SC35" s="0"/>
-      <c r="SD35" s="0"/>
-      <c r="SE35" s="0"/>
-      <c r="SF35" s="0"/>
-      <c r="SG35" s="0"/>
-      <c r="SH35" s="0"/>
-      <c r="SI35" s="0"/>
-      <c r="SJ35" s="0"/>
-      <c r="SK35" s="0"/>
-      <c r="SL35" s="0"/>
-      <c r="SM35" s="0"/>
-      <c r="SN35" s="0"/>
-      <c r="SO35" s="0"/>
-      <c r="SP35" s="0"/>
-      <c r="SQ35" s="0"/>
-      <c r="SR35" s="0"/>
-      <c r="SS35" s="0"/>
-      <c r="ST35" s="0"/>
-      <c r="SU35" s="0"/>
-      <c r="SV35" s="0"/>
-      <c r="SW35" s="0"/>
-      <c r="SX35" s="0"/>
-      <c r="SY35" s="0"/>
-      <c r="SZ35" s="0"/>
-      <c r="TA35" s="0"/>
-      <c r="TB35" s="0"/>
-      <c r="TC35" s="0"/>
-      <c r="TD35" s="0"/>
-      <c r="TE35" s="0"/>
-      <c r="TF35" s="0"/>
-      <c r="TG35" s="0"/>
-      <c r="TH35" s="0"/>
-      <c r="TI35" s="0"/>
-      <c r="TJ35" s="0"/>
-      <c r="TK35" s="0"/>
-      <c r="TL35" s="0"/>
-      <c r="TM35" s="0"/>
-      <c r="TN35" s="0"/>
-      <c r="TO35" s="0"/>
-      <c r="TP35" s="0"/>
-      <c r="TQ35" s="0"/>
-      <c r="TR35" s="0"/>
-      <c r="TS35" s="0"/>
-      <c r="TT35" s="0"/>
-      <c r="TU35" s="0"/>
-      <c r="TV35" s="0"/>
-      <c r="TW35" s="0"/>
-      <c r="TX35" s="0"/>
-      <c r="TY35" s="0"/>
-      <c r="TZ35" s="0"/>
-      <c r="UA35" s="0"/>
-      <c r="UB35" s="0"/>
-      <c r="UC35" s="0"/>
-      <c r="UD35" s="0"/>
-      <c r="UE35" s="0"/>
-      <c r="UF35" s="0"/>
-      <c r="UG35" s="0"/>
-      <c r="UH35" s="0"/>
-      <c r="UI35" s="0"/>
-      <c r="UJ35" s="0"/>
-      <c r="UK35" s="0"/>
-      <c r="UL35" s="0"/>
-      <c r="UM35" s="0"/>
-      <c r="UN35" s="0"/>
-      <c r="UO35" s="0"/>
-      <c r="UP35" s="0"/>
-      <c r="UQ35" s="0"/>
-      <c r="UR35" s="0"/>
-      <c r="US35" s="0"/>
-      <c r="UT35" s="0"/>
-      <c r="UU35" s="0"/>
-      <c r="UV35" s="0"/>
-      <c r="UW35" s="0"/>
-      <c r="UX35" s="0"/>
-      <c r="UY35" s="0"/>
-      <c r="UZ35" s="0"/>
-      <c r="VA35" s="0"/>
-      <c r="VB35" s="0"/>
-      <c r="VC35" s="0"/>
-      <c r="VD35" s="0"/>
-      <c r="VE35" s="0"/>
-      <c r="VF35" s="0"/>
-      <c r="VG35" s="0"/>
-      <c r="VH35" s="0"/>
-      <c r="VI35" s="0"/>
-      <c r="VJ35" s="0"/>
-      <c r="VK35" s="0"/>
-      <c r="VL35" s="0"/>
-      <c r="VM35" s="0"/>
-      <c r="VN35" s="0"/>
-      <c r="VO35" s="0"/>
-      <c r="VP35" s="0"/>
-      <c r="VQ35" s="0"/>
-      <c r="VR35" s="0"/>
-      <c r="VS35" s="0"/>
-      <c r="VT35" s="0"/>
-      <c r="VU35" s="0"/>
-      <c r="VV35" s="0"/>
-      <c r="VW35" s="0"/>
-      <c r="VX35" s="0"/>
-      <c r="VY35" s="0"/>
-      <c r="VZ35" s="0"/>
-      <c r="WA35" s="0"/>
-      <c r="WB35" s="0"/>
-      <c r="WC35" s="0"/>
-      <c r="WD35" s="0"/>
-      <c r="WE35" s="0"/>
-      <c r="WF35" s="0"/>
-      <c r="WG35" s="0"/>
-      <c r="WH35" s="0"/>
-      <c r="WI35" s="0"/>
-      <c r="WJ35" s="0"/>
-      <c r="WK35" s="0"/>
-      <c r="WL35" s="0"/>
-      <c r="WM35" s="0"/>
-      <c r="WN35" s="0"/>
-      <c r="WO35" s="0"/>
-      <c r="WP35" s="0"/>
-      <c r="WQ35" s="0"/>
-      <c r="WR35" s="0"/>
-      <c r="WS35" s="0"/>
-      <c r="WT35" s="0"/>
-      <c r="WU35" s="0"/>
-      <c r="WV35" s="0"/>
-      <c r="WW35" s="0"/>
-      <c r="WX35" s="0"/>
-      <c r="WY35" s="0"/>
-      <c r="WZ35" s="0"/>
-      <c r="XA35" s="0"/>
-      <c r="XB35" s="0"/>
-      <c r="XC35" s="0"/>
-      <c r="XD35" s="0"/>
-      <c r="XE35" s="0"/>
-      <c r="XF35" s="0"/>
-      <c r="XG35" s="0"/>
-      <c r="XH35" s="0"/>
-      <c r="XI35" s="0"/>
-      <c r="XJ35" s="0"/>
-      <c r="XK35" s="0"/>
-      <c r="XL35" s="0"/>
-      <c r="XM35" s="0"/>
-      <c r="XN35" s="0"/>
-      <c r="XO35" s="0"/>
-      <c r="XP35" s="0"/>
-      <c r="XQ35" s="0"/>
-      <c r="XR35" s="0"/>
-      <c r="XS35" s="0"/>
-      <c r="XT35" s="0"/>
-      <c r="XU35" s="0"/>
-      <c r="XV35" s="0"/>
-      <c r="XW35" s="0"/>
-      <c r="XX35" s="0"/>
-      <c r="XY35" s="0"/>
-      <c r="XZ35" s="0"/>
-      <c r="YA35" s="0"/>
-      <c r="YB35" s="0"/>
-      <c r="YC35" s="0"/>
-      <c r="YD35" s="0"/>
-      <c r="YE35" s="0"/>
-      <c r="YF35" s="0"/>
-      <c r="YG35" s="0"/>
-      <c r="YH35" s="0"/>
-      <c r="YI35" s="0"/>
-      <c r="YJ35" s="0"/>
-      <c r="YK35" s="0"/>
-      <c r="YL35" s="0"/>
-      <c r="YM35" s="0"/>
-      <c r="YN35" s="0"/>
-      <c r="YO35" s="0"/>
-      <c r="YP35" s="0"/>
-      <c r="YQ35" s="0"/>
-      <c r="YR35" s="0"/>
-      <c r="YS35" s="0"/>
-      <c r="YT35" s="0"/>
-      <c r="YU35" s="0"/>
-      <c r="YV35" s="0"/>
-      <c r="YW35" s="0"/>
-      <c r="YX35" s="0"/>
-      <c r="YY35" s="0"/>
-      <c r="YZ35" s="0"/>
-      <c r="ZA35" s="0"/>
-      <c r="ZB35" s="0"/>
-      <c r="ZC35" s="0"/>
-      <c r="ZD35" s="0"/>
-      <c r="ZE35" s="0"/>
-      <c r="ZF35" s="0"/>
-      <c r="ZG35" s="0"/>
-      <c r="ZH35" s="0"/>
-      <c r="ZI35" s="0"/>
-      <c r="ZJ35" s="0"/>
-      <c r="ZK35" s="0"/>
-      <c r="ZL35" s="0"/>
-      <c r="ZM35" s="0"/>
-      <c r="ZN35" s="0"/>
-      <c r="ZO35" s="0"/>
-      <c r="ZP35" s="0"/>
-      <c r="ZQ35" s="0"/>
-      <c r="ZR35" s="0"/>
-      <c r="ZS35" s="0"/>
-      <c r="ZT35" s="0"/>
-      <c r="ZU35" s="0"/>
-      <c r="ZV35" s="0"/>
-      <c r="ZW35" s="0"/>
-      <c r="ZX35" s="0"/>
-      <c r="ZY35" s="0"/>
-      <c r="ZZ35" s="0"/>
-      <c r="AAA35" s="0"/>
-      <c r="AAB35" s="0"/>
-      <c r="AAC35" s="0"/>
-      <c r="AAD35" s="0"/>
-      <c r="AAE35" s="0"/>
-      <c r="AAF35" s="0"/>
-      <c r="AAG35" s="0"/>
-      <c r="AAH35" s="0"/>
-      <c r="AAI35" s="0"/>
-      <c r="AAJ35" s="0"/>
-      <c r="AAK35" s="0"/>
-      <c r="AAL35" s="0"/>
-      <c r="AAM35" s="0"/>
-      <c r="AAN35" s="0"/>
-      <c r="AAO35" s="0"/>
-      <c r="AAP35" s="0"/>
-      <c r="AAQ35" s="0"/>
-      <c r="AAR35" s="0"/>
-      <c r="AAS35" s="0"/>
-      <c r="AAT35" s="0"/>
-      <c r="AAU35" s="0"/>
-      <c r="AAV35" s="0"/>
-      <c r="AAW35" s="0"/>
-      <c r="AAX35" s="0"/>
-      <c r="AAY35" s="0"/>
-      <c r="AAZ35" s="0"/>
-      <c r="ABA35" s="0"/>
-      <c r="ABB35" s="0"/>
-      <c r="ABC35" s="0"/>
-      <c r="ABD35" s="0"/>
-      <c r="ABE35" s="0"/>
-      <c r="ABF35" s="0"/>
-      <c r="ABG35" s="0"/>
-      <c r="ABH35" s="0"/>
-      <c r="ABI35" s="0"/>
-      <c r="ABJ35" s="0"/>
-      <c r="ABK35" s="0"/>
-      <c r="ABL35" s="0"/>
-      <c r="ABM35" s="0"/>
-      <c r="ABN35" s="0"/>
-      <c r="ABO35" s="0"/>
-      <c r="ABP35" s="0"/>
-      <c r="ABQ35" s="0"/>
-      <c r="ABR35" s="0"/>
-      <c r="ABS35" s="0"/>
-      <c r="ABT35" s="0"/>
-      <c r="ABU35" s="0"/>
-      <c r="ABV35" s="0"/>
-      <c r="ABW35" s="0"/>
-      <c r="ABX35" s="0"/>
-      <c r="ABY35" s="0"/>
-      <c r="ABZ35" s="0"/>
-      <c r="ACA35" s="0"/>
-      <c r="ACB35" s="0"/>
-      <c r="ACC35" s="0"/>
-      <c r="ACD35" s="0"/>
-      <c r="ACE35" s="0"/>
-      <c r="ACF35" s="0"/>
-      <c r="ACG35" s="0"/>
-      <c r="ACH35" s="0"/>
-      <c r="ACI35" s="0"/>
-      <c r="ACJ35" s="0"/>
-      <c r="ACK35" s="0"/>
-      <c r="ACL35" s="0"/>
-      <c r="ACM35" s="0"/>
-      <c r="ACN35" s="0"/>
-      <c r="ACO35" s="0"/>
-      <c r="ACP35" s="0"/>
-      <c r="ACQ35" s="0"/>
-      <c r="ACR35" s="0"/>
-      <c r="ACS35" s="0"/>
-      <c r="ACT35" s="0"/>
-      <c r="ACU35" s="0"/>
-      <c r="ACV35" s="0"/>
-      <c r="ACW35" s="0"/>
-      <c r="ACX35" s="0"/>
-      <c r="ACY35" s="0"/>
-      <c r="ACZ35" s="0"/>
-      <c r="ADA35" s="0"/>
-      <c r="ADB35" s="0"/>
-      <c r="ADC35" s="0"/>
-      <c r="ADD35" s="0"/>
-      <c r="ADE35" s="0"/>
-      <c r="ADF35" s="0"/>
-      <c r="ADG35" s="0"/>
-      <c r="ADH35" s="0"/>
-      <c r="ADI35" s="0"/>
-      <c r="ADJ35" s="0"/>
-      <c r="ADK35" s="0"/>
-      <c r="ADL35" s="0"/>
-      <c r="ADM35" s="0"/>
-      <c r="ADN35" s="0"/>
-      <c r="ADO35" s="0"/>
-      <c r="ADP35" s="0"/>
-      <c r="ADQ35" s="0"/>
-      <c r="ADR35" s="0"/>
-      <c r="ADS35" s="0"/>
-      <c r="ADT35" s="0"/>
-      <c r="ADU35" s="0"/>
-      <c r="ADV35" s="0"/>
-      <c r="ADW35" s="0"/>
-      <c r="ADX35" s="0"/>
-      <c r="ADY35" s="0"/>
-      <c r="ADZ35" s="0"/>
-      <c r="AEA35" s="0"/>
-      <c r="AEB35" s="0"/>
-      <c r="AEC35" s="0"/>
-      <c r="AED35" s="0"/>
-      <c r="AEE35" s="0"/>
-      <c r="AEF35" s="0"/>
-      <c r="AEG35" s="0"/>
-      <c r="AEH35" s="0"/>
-      <c r="AEI35" s="0"/>
-      <c r="AEJ35" s="0"/>
-      <c r="AEK35" s="0"/>
-      <c r="AEL35" s="0"/>
-      <c r="AEM35" s="0"/>
-      <c r="AEN35" s="0"/>
-      <c r="AEO35" s="0"/>
-      <c r="AEP35" s="0"/>
-      <c r="AEQ35" s="0"/>
-      <c r="AER35" s="0"/>
-      <c r="AES35" s="0"/>
-      <c r="AET35" s="0"/>
-      <c r="AEU35" s="0"/>
-      <c r="AEV35" s="0"/>
-      <c r="AEW35" s="0"/>
-      <c r="AEX35" s="0"/>
-      <c r="AEY35" s="0"/>
-      <c r="AEZ35" s="0"/>
-      <c r="AFA35" s="0"/>
-      <c r="AFB35" s="0"/>
-      <c r="AFC35" s="0"/>
-      <c r="AFD35" s="0"/>
-      <c r="AFE35" s="0"/>
-      <c r="AFF35" s="0"/>
-      <c r="AFG35" s="0"/>
-      <c r="AFH35" s="0"/>
-      <c r="AFI35" s="0"/>
-      <c r="AFJ35" s="0"/>
-      <c r="AFK35" s="0"/>
-      <c r="AFL35" s="0"/>
-      <c r="AFM35" s="0"/>
-      <c r="AFN35" s="0"/>
-      <c r="AFO35" s="0"/>
-      <c r="AFP35" s="0"/>
-      <c r="AFQ35" s="0"/>
-      <c r="AFR35" s="0"/>
-      <c r="AFS35" s="0"/>
-      <c r="AFT35" s="0"/>
-      <c r="AFU35" s="0"/>
-      <c r="AFV35" s="0"/>
-      <c r="AFW35" s="0"/>
-      <c r="AFX35" s="0"/>
-      <c r="AFY35" s="0"/>
-      <c r="AFZ35" s="0"/>
-      <c r="AGA35" s="0"/>
-      <c r="AGB35" s="0"/>
-      <c r="AGC35" s="0"/>
-      <c r="AGD35" s="0"/>
-      <c r="AGE35" s="0"/>
-      <c r="AGF35" s="0"/>
-      <c r="AGG35" s="0"/>
-      <c r="AGH35" s="0"/>
-      <c r="AGI35" s="0"/>
-      <c r="AGJ35" s="0"/>
-      <c r="AGK35" s="0"/>
-      <c r="AGL35" s="0"/>
-      <c r="AGM35" s="0"/>
-      <c r="AGN35" s="0"/>
-      <c r="AGO35" s="0"/>
-      <c r="AGP35" s="0"/>
-      <c r="AGQ35" s="0"/>
-      <c r="AGR35" s="0"/>
-      <c r="AGS35" s="0"/>
-      <c r="AGT35" s="0"/>
-      <c r="AGU35" s="0"/>
-      <c r="AGV35" s="0"/>
-      <c r="AGW35" s="0"/>
-      <c r="AGX35" s="0"/>
-      <c r="AGY35" s="0"/>
-      <c r="AGZ35" s="0"/>
-      <c r="AHA35" s="0"/>
-      <c r="AHB35" s="0"/>
-      <c r="AHC35" s="0"/>
-      <c r="AHD35" s="0"/>
-      <c r="AHE35" s="0"/>
-      <c r="AHF35" s="0"/>
-      <c r="AHG35" s="0"/>
-      <c r="AHH35" s="0"/>
-      <c r="AHI35" s="0"/>
-      <c r="AHJ35" s="0"/>
-      <c r="AHK35" s="0"/>
-      <c r="AHL35" s="0"/>
-      <c r="AHM35" s="0"/>
-      <c r="AHN35" s="0"/>
-      <c r="AHO35" s="0"/>
-      <c r="AHP35" s="0"/>
-      <c r="AHQ35" s="0"/>
-      <c r="AHR35" s="0"/>
-      <c r="AHS35" s="0"/>
-      <c r="AHT35" s="0"/>
-      <c r="AHU35" s="0"/>
-      <c r="AHV35" s="0"/>
-      <c r="AHW35" s="0"/>
-      <c r="AHX35" s="0"/>
-      <c r="AHY35" s="0"/>
-      <c r="AHZ35" s="0"/>
-      <c r="AIA35" s="0"/>
-      <c r="AIB35" s="0"/>
-      <c r="AIC35" s="0"/>
-      <c r="AID35" s="0"/>
-      <c r="AIE35" s="0"/>
-      <c r="AIF35" s="0"/>
-      <c r="AIG35" s="0"/>
-      <c r="AIH35" s="0"/>
-      <c r="AII35" s="0"/>
-      <c r="AIJ35" s="0"/>
-      <c r="AIK35" s="0"/>
-      <c r="AIL35" s="0"/>
-      <c r="AIM35" s="0"/>
-      <c r="AIN35" s="0"/>
-      <c r="AIO35" s="0"/>
-      <c r="AIP35" s="0"/>
-      <c r="AIQ35" s="0"/>
-      <c r="AIR35" s="0"/>
-      <c r="AIS35" s="0"/>
-      <c r="AIT35" s="0"/>
-      <c r="AIU35" s="0"/>
-      <c r="AIV35" s="0"/>
-      <c r="AIW35" s="0"/>
-      <c r="AIX35" s="0"/>
-      <c r="AIY35" s="0"/>
-      <c r="AIZ35" s="0"/>
-      <c r="AJA35" s="0"/>
-      <c r="AJB35" s="0"/>
-      <c r="AJC35" s="0"/>
-      <c r="AJD35" s="0"/>
-      <c r="AJE35" s="0"/>
-      <c r="AJF35" s="0"/>
-      <c r="AJG35" s="0"/>
-      <c r="AJH35" s="0"/>
-      <c r="AJI35" s="0"/>
-      <c r="AJJ35" s="0"/>
-      <c r="AJK35" s="0"/>
-      <c r="AJL35" s="0"/>
-      <c r="AJM35" s="0"/>
-      <c r="AJN35" s="0"/>
-      <c r="AJO35" s="0"/>
-      <c r="AJP35" s="0"/>
-      <c r="AJQ35" s="0"/>
-      <c r="AJR35" s="0"/>
-      <c r="AJS35" s="0"/>
-      <c r="AJT35" s="0"/>
-      <c r="AJU35" s="0"/>
-      <c r="AJV35" s="0"/>
-      <c r="AJW35" s="0"/>
-      <c r="AJX35" s="0"/>
-      <c r="AJY35" s="0"/>
-      <c r="AJZ35" s="0"/>
-      <c r="AKA35" s="0"/>
-      <c r="AKB35" s="0"/>
-      <c r="AKC35" s="0"/>
-      <c r="AKD35" s="0"/>
-      <c r="AKE35" s="0"/>
-      <c r="AKF35" s="0"/>
-      <c r="AKG35" s="0"/>
-      <c r="AKH35" s="0"/>
-      <c r="AKI35" s="0"/>
-      <c r="AKJ35" s="0"/>
-      <c r="AKK35" s="0"/>
-      <c r="AKL35" s="0"/>
-      <c r="AKM35" s="0"/>
-      <c r="AKN35" s="0"/>
-      <c r="AKO35" s="0"/>
-      <c r="AKP35" s="0"/>
-      <c r="AKQ35" s="0"/>
-      <c r="AKR35" s="0"/>
-      <c r="AKS35" s="0"/>
-      <c r="AKT35" s="0"/>
-      <c r="AKU35" s="0"/>
-      <c r="AKV35" s="0"/>
-      <c r="AKW35" s="0"/>
-      <c r="AKX35" s="0"/>
-      <c r="AKY35" s="0"/>
-      <c r="AKZ35" s="0"/>
-      <c r="ALA35" s="0"/>
-      <c r="ALB35" s="0"/>
-      <c r="ALC35" s="0"/>
-      <c r="ALD35" s="0"/>
-      <c r="ALE35" s="0"/>
-      <c r="ALF35" s="0"/>
-      <c r="ALG35" s="0"/>
-      <c r="ALH35" s="0"/>
-      <c r="ALI35" s="0"/>
-      <c r="ALJ35" s="0"/>
-      <c r="ALK35" s="0"/>
-      <c r="ALL35" s="0"/>
-      <c r="ALM35" s="0"/>
-      <c r="ALN35" s="0"/>
-      <c r="ALO35" s="0"/>
-      <c r="ALP35" s="0"/>
-      <c r="ALQ35" s="0"/>
-      <c r="ALR35" s="0"/>
-      <c r="ALS35" s="0"/>
-      <c r="ALT35" s="0"/>
-      <c r="ALU35" s="0"/>
-      <c r="ALV35" s="0"/>
-      <c r="ALW35" s="0"/>
-      <c r="ALX35" s="0"/>
-      <c r="ALY35" s="0"/>
-      <c r="ALZ35" s="0"/>
-      <c r="AMA35" s="0"/>
-      <c r="AMB35" s="0"/>
-      <c r="AMC35" s="0"/>
-      <c r="AMD35" s="0"/>
-      <c r="AME35" s="0"/>
-      <c r="AMF35" s="0"/>
-      <c r="AMG35" s="0"/>
-      <c r="AMH35" s="0"/>
-      <c r="AMI35" s="0"/>
-      <c r="AMJ35" s="0"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="0"/>
-      <c r="O36" s="0"/>
-      <c r="P36" s="0"/>
-      <c r="Q36" s="0"/>
-      <c r="R36" s="0"/>
-      <c r="S36" s="0"/>
-      <c r="T36" s="0"/>
-      <c r="U36" s="0"/>
-      <c r="V36" s="0"/>
-      <c r="W36" s="0"/>
-      <c r="X36" s="0"/>
-      <c r="Y36" s="0"/>
-      <c r="Z36" s="0"/>
-      <c r="AA36" s="0"/>
-      <c r="AB36" s="0"/>
-      <c r="AC36" s="0"/>
-      <c r="AD36" s="0"/>
-      <c r="AE36" s="0"/>
-      <c r="AF36" s="0"/>
-      <c r="AG36" s="0"/>
-      <c r="AH36" s="0"/>
-      <c r="AI36" s="0"/>
-      <c r="AJ36" s="0"/>
-      <c r="AK36" s="0"/>
-      <c r="AL36" s="0"/>
-      <c r="AM36" s="0"/>
-      <c r="AN36" s="0"/>
-      <c r="AO36" s="0"/>
-      <c r="AP36" s="0"/>
-      <c r="AQ36" s="0"/>
-      <c r="AR36" s="0"/>
-      <c r="AS36" s="0"/>
-      <c r="AT36" s="0"/>
-      <c r="AU36" s="0"/>
-      <c r="AV36" s="0"/>
-      <c r="AW36" s="0"/>
-      <c r="AX36" s="0"/>
-      <c r="AY36" s="0"/>
-      <c r="AZ36" s="0"/>
-      <c r="BA36" s="0"/>
-      <c r="BB36" s="0"/>
-      <c r="BC36" s="0"/>
-      <c r="BD36" s="0"/>
-      <c r="BE36" s="0"/>
-      <c r="BF36" s="0"/>
-      <c r="BG36" s="0"/>
-      <c r="BH36" s="0"/>
-      <c r="BI36" s="0"/>
-      <c r="BJ36" s="0"/>
-      <c r="BK36" s="0"/>
-      <c r="BL36" s="0"/>
-      <c r="BM36" s="0"/>
-      <c r="BN36" s="0"/>
-      <c r="BO36" s="0"/>
-      <c r="BP36" s="0"/>
-      <c r="BQ36" s="0"/>
-      <c r="BR36" s="0"/>
-      <c r="BS36" s="0"/>
-      <c r="BT36" s="0"/>
-      <c r="BU36" s="0"/>
-      <c r="BV36" s="0"/>
-      <c r="BW36" s="0"/>
-      <c r="BX36" s="0"/>
-      <c r="BY36" s="0"/>
-      <c r="BZ36" s="0"/>
-      <c r="CA36" s="0"/>
-      <c r="CB36" s="0"/>
-      <c r="CC36" s="0"/>
-      <c r="CD36" s="0"/>
-      <c r="CE36" s="0"/>
-      <c r="CF36" s="0"/>
-      <c r="CG36" s="0"/>
-      <c r="CH36" s="0"/>
-      <c r="CI36" s="0"/>
-      <c r="CJ36" s="0"/>
-      <c r="CK36" s="0"/>
-      <c r="CL36" s="0"/>
-      <c r="CM36" s="0"/>
-      <c r="CN36" s="0"/>
-      <c r="CO36" s="0"/>
-      <c r="CP36" s="0"/>
-      <c r="CQ36" s="0"/>
-      <c r="CR36" s="0"/>
-      <c r="CS36" s="0"/>
-      <c r="CT36" s="0"/>
-      <c r="CU36" s="0"/>
-      <c r="CV36" s="0"/>
-      <c r="CW36" s="0"/>
-      <c r="CX36" s="0"/>
-      <c r="CY36" s="0"/>
-      <c r="CZ36" s="0"/>
-      <c r="DA36" s="0"/>
-      <c r="DB36" s="0"/>
-      <c r="DC36" s="0"/>
-      <c r="DD36" s="0"/>
-      <c r="DE36" s="0"/>
-      <c r="DF36" s="0"/>
-      <c r="DG36" s="0"/>
-      <c r="DH36" s="0"/>
-      <c r="DI36" s="0"/>
-      <c r="DJ36" s="0"/>
-      <c r="DK36" s="0"/>
-      <c r="DL36" s="0"/>
-      <c r="DM36" s="0"/>
-      <c r="DN36" s="0"/>
-      <c r="DO36" s="0"/>
-      <c r="DP36" s="0"/>
-      <c r="DQ36" s="0"/>
-      <c r="DR36" s="0"/>
-      <c r="DS36" s="0"/>
-      <c r="DT36" s="0"/>
-      <c r="DU36" s="0"/>
-      <c r="DV36" s="0"/>
-      <c r="DW36" s="0"/>
-      <c r="DX36" s="0"/>
-      <c r="DY36" s="0"/>
-      <c r="DZ36" s="0"/>
-      <c r="EA36" s="0"/>
-      <c r="EB36" s="0"/>
-      <c r="EC36" s="0"/>
-      <c r="ED36" s="0"/>
-      <c r="EE36" s="0"/>
-      <c r="EF36" s="0"/>
-      <c r="EG36" s="0"/>
-      <c r="EH36" s="0"/>
-      <c r="EI36" s="0"/>
-      <c r="EJ36" s="0"/>
-      <c r="EK36" s="0"/>
-      <c r="EL36" s="0"/>
-      <c r="EM36" s="0"/>
-      <c r="EN36" s="0"/>
-      <c r="EO36" s="0"/>
-      <c r="EP36" s="0"/>
-      <c r="EQ36" s="0"/>
-      <c r="ER36" s="0"/>
-      <c r="ES36" s="0"/>
-      <c r="ET36" s="0"/>
-      <c r="EU36" s="0"/>
-      <c r="EV36" s="0"/>
-      <c r="EW36" s="0"/>
-      <c r="EX36" s="0"/>
-      <c r="EY36" s="0"/>
-      <c r="EZ36" s="0"/>
-      <c r="FA36" s="0"/>
-      <c r="FB36" s="0"/>
-      <c r="FC36" s="0"/>
-      <c r="FD36" s="0"/>
-      <c r="FE36" s="0"/>
-      <c r="FF36" s="0"/>
-      <c r="FG36" s="0"/>
-      <c r="FH36" s="0"/>
-      <c r="FI36" s="0"/>
-      <c r="FJ36" s="0"/>
-      <c r="FK36" s="0"/>
-      <c r="FL36" s="0"/>
-      <c r="FM36" s="0"/>
-      <c r="FN36" s="0"/>
-      <c r="FO36" s="0"/>
-      <c r="FP36" s="0"/>
-      <c r="FQ36" s="0"/>
-      <c r="FR36" s="0"/>
-      <c r="FS36" s="0"/>
-      <c r="FT36" s="0"/>
-      <c r="FU36" s="0"/>
-      <c r="FV36" s="0"/>
-      <c r="FW36" s="0"/>
-      <c r="FX36" s="0"/>
-      <c r="FY36" s="0"/>
-      <c r="FZ36" s="0"/>
-      <c r="GA36" s="0"/>
-      <c r="GB36" s="0"/>
-      <c r="GC36" s="0"/>
-      <c r="GD36" s="0"/>
-      <c r="GE36" s="0"/>
-      <c r="GF36" s="0"/>
-      <c r="GG36" s="0"/>
-      <c r="GH36" s="0"/>
-      <c r="GI36" s="0"/>
-      <c r="GJ36" s="0"/>
-      <c r="GK36" s="0"/>
-      <c r="GL36" s="0"/>
-      <c r="GM36" s="0"/>
-      <c r="GN36" s="0"/>
-      <c r="GO36" s="0"/>
-      <c r="GP36" s="0"/>
-      <c r="GQ36" s="0"/>
-      <c r="GR36" s="0"/>
-      <c r="GS36" s="0"/>
-      <c r="GT36" s="0"/>
-      <c r="GU36" s="0"/>
-      <c r="GV36" s="0"/>
-      <c r="GW36" s="0"/>
-      <c r="GX36" s="0"/>
-      <c r="GY36" s="0"/>
-      <c r="GZ36" s="0"/>
-      <c r="HA36" s="0"/>
-      <c r="HB36" s="0"/>
-      <c r="HC36" s="0"/>
-      <c r="HD36" s="0"/>
-      <c r="HE36" s="0"/>
-      <c r="HF36" s="0"/>
-      <c r="HG36" s="0"/>
-      <c r="HH36" s="0"/>
-      <c r="HI36" s="0"/>
-      <c r="HJ36" s="0"/>
-      <c r="HK36" s="0"/>
-      <c r="HL36" s="0"/>
-      <c r="HM36" s="0"/>
-      <c r="HN36" s="0"/>
-      <c r="HO36" s="0"/>
-      <c r="HP36" s="0"/>
-      <c r="HQ36" s="0"/>
-      <c r="HR36" s="0"/>
-      <c r="HS36" s="0"/>
-      <c r="HT36" s="0"/>
-      <c r="HU36" s="0"/>
-      <c r="HV36" s="0"/>
-      <c r="HW36" s="0"/>
-      <c r="HX36" s="0"/>
-      <c r="HY36" s="0"/>
-      <c r="HZ36" s="0"/>
-      <c r="IA36" s="0"/>
-      <c r="IB36" s="0"/>
-      <c r="IC36" s="0"/>
-      <c r="ID36" s="0"/>
-      <c r="IE36" s="0"/>
-      <c r="IF36" s="0"/>
-      <c r="IG36" s="0"/>
-      <c r="IH36" s="0"/>
-      <c r="II36" s="0"/>
-      <c r="IJ36" s="0"/>
-      <c r="IK36" s="0"/>
-      <c r="IL36" s="0"/>
-      <c r="IM36" s="0"/>
-      <c r="IN36" s="0"/>
-      <c r="IO36" s="0"/>
-      <c r="IP36" s="0"/>
-      <c r="IQ36" s="0"/>
-      <c r="IR36" s="0"/>
-      <c r="IS36" s="0"/>
-      <c r="IT36" s="0"/>
-      <c r="IU36" s="0"/>
-      <c r="IV36" s="0"/>
-      <c r="IW36" s="0"/>
-      <c r="IX36" s="0"/>
-      <c r="IY36" s="0"/>
-      <c r="IZ36" s="0"/>
-      <c r="JA36" s="0"/>
-      <c r="JB36" s="0"/>
-      <c r="JC36" s="0"/>
-      <c r="JD36" s="0"/>
-      <c r="JE36" s="0"/>
-      <c r="JF36" s="0"/>
-      <c r="JG36" s="0"/>
-      <c r="JH36" s="0"/>
-      <c r="JI36" s="0"/>
-      <c r="JJ36" s="0"/>
-      <c r="JK36" s="0"/>
-      <c r="JL36" s="0"/>
-      <c r="JM36" s="0"/>
-      <c r="JN36" s="0"/>
-      <c r="JO36" s="0"/>
-      <c r="JP36" s="0"/>
-      <c r="JQ36" s="0"/>
-      <c r="JR36" s="0"/>
-      <c r="JS36" s="0"/>
-      <c r="JT36" s="0"/>
-      <c r="JU36" s="0"/>
-      <c r="JV36" s="0"/>
-      <c r="JW36" s="0"/>
-      <c r="JX36" s="0"/>
-      <c r="JY36" s="0"/>
-      <c r="JZ36" s="0"/>
-      <c r="KA36" s="0"/>
-      <c r="KB36" s="0"/>
-      <c r="KC36" s="0"/>
-      <c r="KD36" s="0"/>
-      <c r="KE36" s="0"/>
-      <c r="KF36" s="0"/>
-      <c r="KG36" s="0"/>
-      <c r="KH36" s="0"/>
-      <c r="KI36" s="0"/>
-      <c r="KJ36" s="0"/>
-      <c r="KK36" s="0"/>
-      <c r="KL36" s="0"/>
-      <c r="KM36" s="0"/>
-      <c r="KN36" s="0"/>
-      <c r="KO36" s="0"/>
-      <c r="KP36" s="0"/>
-      <c r="KQ36" s="0"/>
-      <c r="KR36" s="0"/>
-      <c r="KS36" s="0"/>
-      <c r="KT36" s="0"/>
-      <c r="KU36" s="0"/>
-      <c r="KV36" s="0"/>
-      <c r="KW36" s="0"/>
-      <c r="KX36" s="0"/>
-      <c r="KY36" s="0"/>
-      <c r="KZ36" s="0"/>
-      <c r="LA36" s="0"/>
-      <c r="LB36" s="0"/>
-      <c r="LC36" s="0"/>
-      <c r="LD36" s="0"/>
-      <c r="LE36" s="0"/>
-      <c r="LF36" s="0"/>
-      <c r="LG36" s="0"/>
-      <c r="LH36" s="0"/>
-      <c r="LI36" s="0"/>
-      <c r="LJ36" s="0"/>
-      <c r="LK36" s="0"/>
-      <c r="LL36" s="0"/>
-      <c r="LM36" s="0"/>
-      <c r="LN36" s="0"/>
-      <c r="LO36" s="0"/>
-      <c r="LP36" s="0"/>
-      <c r="LQ36" s="0"/>
-      <c r="LR36" s="0"/>
-      <c r="LS36" s="0"/>
-      <c r="LT36" s="0"/>
-      <c r="LU36" s="0"/>
-      <c r="LV36" s="0"/>
-      <c r="LW36" s="0"/>
-      <c r="LX36" s="0"/>
-      <c r="LY36" s="0"/>
-      <c r="LZ36" s="0"/>
-      <c r="MA36" s="0"/>
-      <c r="MB36" s="0"/>
-      <c r="MC36" s="0"/>
-      <c r="MD36" s="0"/>
-      <c r="ME36" s="0"/>
-      <c r="MF36" s="0"/>
-      <c r="MG36" s="0"/>
-      <c r="MH36" s="0"/>
-      <c r="MI36" s="0"/>
-      <c r="MJ36" s="0"/>
-      <c r="MK36" s="0"/>
-      <c r="ML36" s="0"/>
-      <c r="MM36" s="0"/>
-      <c r="MN36" s="0"/>
-      <c r="MO36" s="0"/>
-      <c r="MP36" s="0"/>
-      <c r="MQ36" s="0"/>
-      <c r="MR36" s="0"/>
-      <c r="MS36" s="0"/>
-      <c r="MT36" s="0"/>
-      <c r="MU36" s="0"/>
-      <c r="MV36" s="0"/>
-      <c r="MW36" s="0"/>
-      <c r="MX36" s="0"/>
-      <c r="MY36" s="0"/>
-      <c r="MZ36" s="0"/>
-      <c r="NA36" s="0"/>
-      <c r="NB36" s="0"/>
-      <c r="NC36" s="0"/>
-      <c r="ND36" s="0"/>
-      <c r="NE36" s="0"/>
-      <c r="NF36" s="0"/>
-      <c r="NG36" s="0"/>
-      <c r="NH36" s="0"/>
-      <c r="NI36" s="0"/>
-      <c r="NJ36" s="0"/>
-      <c r="NK36" s="0"/>
-      <c r="NL36" s="0"/>
-      <c r="NM36" s="0"/>
-      <c r="NN36" s="0"/>
-      <c r="NO36" s="0"/>
-      <c r="NP36" s="0"/>
-      <c r="NQ36" s="0"/>
-      <c r="NR36" s="0"/>
-      <c r="NS36" s="0"/>
-      <c r="NT36" s="0"/>
-      <c r="NU36" s="0"/>
-      <c r="NV36" s="0"/>
-      <c r="NW36" s="0"/>
-      <c r="NX36" s="0"/>
-      <c r="NY36" s="0"/>
-      <c r="NZ36" s="0"/>
-      <c r="OA36" s="0"/>
-      <c r="OB36" s="0"/>
-      <c r="OC36" s="0"/>
-      <c r="OD36" s="0"/>
-      <c r="OE36" s="0"/>
-      <c r="OF36" s="0"/>
-      <c r="OG36" s="0"/>
-      <c r="OH36" s="0"/>
-      <c r="OI36" s="0"/>
-      <c r="OJ36" s="0"/>
-      <c r="OK36" s="0"/>
-      <c r="OL36" s="0"/>
-      <c r="OM36" s="0"/>
-      <c r="ON36" s="0"/>
-      <c r="OO36" s="0"/>
-      <c r="OP36" s="0"/>
-      <c r="OQ36" s="0"/>
-      <c r="OR36" s="0"/>
-      <c r="OS36" s="0"/>
-      <c r="OT36" s="0"/>
-      <c r="OU36" s="0"/>
-      <c r="OV36" s="0"/>
-      <c r="OW36" s="0"/>
-      <c r="OX36" s="0"/>
-      <c r="OY36" s="0"/>
-      <c r="OZ36" s="0"/>
-      <c r="PA36" s="0"/>
-      <c r="PB36" s="0"/>
-      <c r="PC36" s="0"/>
-      <c r="PD36" s="0"/>
-      <c r="PE36" s="0"/>
-      <c r="PF36" s="0"/>
-      <c r="PG36" s="0"/>
-      <c r="PH36" s="0"/>
-      <c r="PI36" s="0"/>
-      <c r="PJ36" s="0"/>
-      <c r="PK36" s="0"/>
-      <c r="PL36" s="0"/>
-      <c r="PM36" s="0"/>
-      <c r="PN36" s="0"/>
-      <c r="PO36" s="0"/>
-      <c r="PP36" s="0"/>
-      <c r="PQ36" s="0"/>
-      <c r="PR36" s="0"/>
-      <c r="PS36" s="0"/>
-      <c r="PT36" s="0"/>
-      <c r="PU36" s="0"/>
-      <c r="PV36" s="0"/>
-      <c r="PW36" s="0"/>
-      <c r="PX36" s="0"/>
-      <c r="PY36" s="0"/>
-      <c r="PZ36" s="0"/>
-      <c r="QA36" s="0"/>
-      <c r="QB36" s="0"/>
-      <c r="QC36" s="0"/>
-      <c r="QD36" s="0"/>
-      <c r="QE36" s="0"/>
-      <c r="QF36" s="0"/>
-      <c r="QG36" s="0"/>
-      <c r="QH36" s="0"/>
-      <c r="QI36" s="0"/>
-      <c r="QJ36" s="0"/>
-      <c r="QK36" s="0"/>
-      <c r="QL36" s="0"/>
-      <c r="QM36" s="0"/>
-      <c r="QN36" s="0"/>
-      <c r="QO36" s="0"/>
-      <c r="QP36" s="0"/>
-      <c r="QQ36" s="0"/>
-      <c r="QR36" s="0"/>
-      <c r="QS36" s="0"/>
-      <c r="QT36" s="0"/>
-      <c r="QU36" s="0"/>
-      <c r="QV36" s="0"/>
-      <c r="QW36" s="0"/>
-      <c r="QX36" s="0"/>
-      <c r="QY36" s="0"/>
-      <c r="QZ36" s="0"/>
-      <c r="RA36" s="0"/>
-      <c r="RB36" s="0"/>
-      <c r="RC36" s="0"/>
-      <c r="RD36" s="0"/>
-      <c r="RE36" s="0"/>
-      <c r="RF36" s="0"/>
-      <c r="RG36" s="0"/>
-      <c r="RH36" s="0"/>
-      <c r="RI36" s="0"/>
-      <c r="RJ36" s="0"/>
-      <c r="RK36" s="0"/>
-      <c r="RL36" s="0"/>
-      <c r="RM36" s="0"/>
-      <c r="RN36" s="0"/>
-      <c r="RO36" s="0"/>
-      <c r="RP36" s="0"/>
-      <c r="RQ36" s="0"/>
-      <c r="RR36" s="0"/>
-      <c r="RS36" s="0"/>
-      <c r="RT36" s="0"/>
-      <c r="RU36" s="0"/>
-      <c r="RV36" s="0"/>
-      <c r="RW36" s="0"/>
-      <c r="RX36" s="0"/>
-      <c r="RY36" s="0"/>
-      <c r="RZ36" s="0"/>
-      <c r="SA36" s="0"/>
-      <c r="SB36" s="0"/>
-      <c r="SC36" s="0"/>
-      <c r="SD36" s="0"/>
-      <c r="SE36" s="0"/>
-      <c r="SF36" s="0"/>
-      <c r="SG36" s="0"/>
-      <c r="SH36" s="0"/>
-      <c r="SI36" s="0"/>
-      <c r="SJ36" s="0"/>
-      <c r="SK36" s="0"/>
-      <c r="SL36" s="0"/>
-      <c r="SM36" s="0"/>
-      <c r="SN36" s="0"/>
-      <c r="SO36" s="0"/>
-      <c r="SP36" s="0"/>
-      <c r="SQ36" s="0"/>
-      <c r="SR36" s="0"/>
-      <c r="SS36" s="0"/>
-      <c r="ST36" s="0"/>
-      <c r="SU36" s="0"/>
-      <c r="SV36" s="0"/>
-      <c r="SW36" s="0"/>
-      <c r="SX36" s="0"/>
-      <c r="SY36" s="0"/>
-      <c r="SZ36" s="0"/>
-      <c r="TA36" s="0"/>
-      <c r="TB36" s="0"/>
-      <c r="TC36" s="0"/>
-      <c r="TD36" s="0"/>
-      <c r="TE36" s="0"/>
-      <c r="TF36" s="0"/>
-      <c r="TG36" s="0"/>
-      <c r="TH36" s="0"/>
-      <c r="TI36" s="0"/>
-      <c r="TJ36" s="0"/>
-      <c r="TK36" s="0"/>
-      <c r="TL36" s="0"/>
-      <c r="TM36" s="0"/>
-      <c r="TN36" s="0"/>
-      <c r="TO36" s="0"/>
-      <c r="TP36" s="0"/>
-      <c r="TQ36" s="0"/>
-      <c r="TR36" s="0"/>
-      <c r="TS36" s="0"/>
-      <c r="TT36" s="0"/>
-      <c r="TU36" s="0"/>
-      <c r="TV36" s="0"/>
-      <c r="TW36" s="0"/>
-      <c r="TX36" s="0"/>
-      <c r="TY36" s="0"/>
-      <c r="TZ36" s="0"/>
-      <c r="UA36" s="0"/>
-      <c r="UB36" s="0"/>
-      <c r="UC36" s="0"/>
-      <c r="UD36" s="0"/>
-      <c r="UE36" s="0"/>
-      <c r="UF36" s="0"/>
-      <c r="UG36" s="0"/>
-      <c r="UH36" s="0"/>
-      <c r="UI36" s="0"/>
-      <c r="UJ36" s="0"/>
-      <c r="UK36" s="0"/>
-      <c r="UL36" s="0"/>
-      <c r="UM36" s="0"/>
-      <c r="UN36" s="0"/>
-      <c r="UO36" s="0"/>
-      <c r="UP36" s="0"/>
-      <c r="UQ36" s="0"/>
-      <c r="UR36" s="0"/>
-      <c r="US36" s="0"/>
-      <c r="UT36" s="0"/>
-      <c r="UU36" s="0"/>
-      <c r="UV36" s="0"/>
-      <c r="UW36" s="0"/>
-      <c r="UX36" s="0"/>
-      <c r="UY36" s="0"/>
-      <c r="UZ36" s="0"/>
-      <c r="VA36" s="0"/>
-      <c r="VB36" s="0"/>
-      <c r="VC36" s="0"/>
-      <c r="VD36" s="0"/>
-      <c r="VE36" s="0"/>
-      <c r="VF36" s="0"/>
-      <c r="VG36" s="0"/>
-      <c r="VH36" s="0"/>
-      <c r="VI36" s="0"/>
-      <c r="VJ36" s="0"/>
-      <c r="VK36" s="0"/>
-      <c r="VL36" s="0"/>
-      <c r="VM36" s="0"/>
-      <c r="VN36" s="0"/>
-      <c r="VO36" s="0"/>
-      <c r="VP36" s="0"/>
-      <c r="VQ36" s="0"/>
-      <c r="VR36" s="0"/>
-      <c r="VS36" s="0"/>
-      <c r="VT36" s="0"/>
-      <c r="VU36" s="0"/>
-      <c r="VV36" s="0"/>
-      <c r="VW36" s="0"/>
-      <c r="VX36" s="0"/>
-      <c r="VY36" s="0"/>
-      <c r="VZ36" s="0"/>
-      <c r="WA36" s="0"/>
-      <c r="WB36" s="0"/>
-      <c r="WC36" s="0"/>
-      <c r="WD36" s="0"/>
-      <c r="WE36" s="0"/>
-      <c r="WF36" s="0"/>
-      <c r="WG36" s="0"/>
-      <c r="WH36" s="0"/>
-      <c r="WI36" s="0"/>
-      <c r="WJ36" s="0"/>
-      <c r="WK36" s="0"/>
-      <c r="WL36" s="0"/>
-      <c r="WM36" s="0"/>
-      <c r="WN36" s="0"/>
-      <c r="WO36" s="0"/>
-      <c r="WP36" s="0"/>
-      <c r="WQ36" s="0"/>
-      <c r="WR36" s="0"/>
-      <c r="WS36" s="0"/>
-      <c r="WT36" s="0"/>
-      <c r="WU36" s="0"/>
-      <c r="WV36" s="0"/>
-      <c r="WW36" s="0"/>
-      <c r="WX36" s="0"/>
-      <c r="WY36" s="0"/>
-      <c r="WZ36" s="0"/>
-      <c r="XA36" s="0"/>
-      <c r="XB36" s="0"/>
-      <c r="XC36" s="0"/>
-      <c r="XD36" s="0"/>
-      <c r="XE36" s="0"/>
-      <c r="XF36" s="0"/>
-      <c r="XG36" s="0"/>
-      <c r="XH36" s="0"/>
-      <c r="XI36" s="0"/>
-      <c r="XJ36" s="0"/>
-      <c r="XK36" s="0"/>
-      <c r="XL36" s="0"/>
-      <c r="XM36" s="0"/>
-      <c r="XN36" s="0"/>
-      <c r="XO36" s="0"/>
-      <c r="XP36" s="0"/>
-      <c r="XQ36" s="0"/>
-      <c r="XR36" s="0"/>
-      <c r="XS36" s="0"/>
-      <c r="XT36" s="0"/>
-      <c r="XU36" s="0"/>
-      <c r="XV36" s="0"/>
-      <c r="XW36" s="0"/>
-      <c r="XX36" s="0"/>
-      <c r="XY36" s="0"/>
-      <c r="XZ36" s="0"/>
-      <c r="YA36" s="0"/>
-      <c r="YB36" s="0"/>
-      <c r="YC36" s="0"/>
-      <c r="YD36" s="0"/>
-      <c r="YE36" s="0"/>
-      <c r="YF36" s="0"/>
-      <c r="YG36" s="0"/>
-      <c r="YH36" s="0"/>
-      <c r="YI36" s="0"/>
-      <c r="YJ36" s="0"/>
-      <c r="YK36" s="0"/>
-      <c r="YL36" s="0"/>
-      <c r="YM36" s="0"/>
-      <c r="YN36" s="0"/>
-      <c r="YO36" s="0"/>
-      <c r="YP36" s="0"/>
-      <c r="YQ36" s="0"/>
-      <c r="YR36" s="0"/>
-      <c r="YS36" s="0"/>
-      <c r="YT36" s="0"/>
-      <c r="YU36" s="0"/>
-      <c r="YV36" s="0"/>
-      <c r="YW36" s="0"/>
-      <c r="YX36" s="0"/>
-      <c r="YY36" s="0"/>
-      <c r="YZ36" s="0"/>
-      <c r="ZA36" s="0"/>
-      <c r="ZB36" s="0"/>
-      <c r="ZC36" s="0"/>
-      <c r="ZD36" s="0"/>
-      <c r="ZE36" s="0"/>
-      <c r="ZF36" s="0"/>
-      <c r="ZG36" s="0"/>
-      <c r="ZH36" s="0"/>
-      <c r="ZI36" s="0"/>
-      <c r="ZJ36" s="0"/>
-      <c r="ZK36" s="0"/>
-      <c r="ZL36" s="0"/>
-      <c r="ZM36" s="0"/>
-      <c r="ZN36" s="0"/>
-      <c r="ZO36" s="0"/>
-      <c r="ZP36" s="0"/>
-      <c r="ZQ36" s="0"/>
-      <c r="ZR36" s="0"/>
-      <c r="ZS36" s="0"/>
-      <c r="ZT36" s="0"/>
-      <c r="ZU36" s="0"/>
-      <c r="ZV36" s="0"/>
-      <c r="ZW36" s="0"/>
-      <c r="ZX36" s="0"/>
-      <c r="ZY36" s="0"/>
-      <c r="ZZ36" s="0"/>
-      <c r="AAA36" s="0"/>
-      <c r="AAB36" s="0"/>
-      <c r="AAC36" s="0"/>
-      <c r="AAD36" s="0"/>
-      <c r="AAE36" s="0"/>
-      <c r="AAF36" s="0"/>
-      <c r="AAG36" s="0"/>
-      <c r="AAH36" s="0"/>
-      <c r="AAI36" s="0"/>
-      <c r="AAJ36" s="0"/>
-      <c r="AAK36" s="0"/>
-      <c r="AAL36" s="0"/>
-      <c r="AAM36" s="0"/>
-      <c r="AAN36" s="0"/>
-      <c r="AAO36" s="0"/>
-      <c r="AAP36" s="0"/>
-      <c r="AAQ36" s="0"/>
-      <c r="AAR36" s="0"/>
-      <c r="AAS36" s="0"/>
-      <c r="AAT36" s="0"/>
-      <c r="AAU36" s="0"/>
-      <c r="AAV36" s="0"/>
-      <c r="AAW36" s="0"/>
-      <c r="AAX36" s="0"/>
-      <c r="AAY36" s="0"/>
-      <c r="AAZ36" s="0"/>
-      <c r="ABA36" s="0"/>
-      <c r="ABB36" s="0"/>
-      <c r="ABC36" s="0"/>
-      <c r="ABD36" s="0"/>
-      <c r="ABE36" s="0"/>
-      <c r="ABF36" s="0"/>
-      <c r="ABG36" s="0"/>
-      <c r="ABH36" s="0"/>
-      <c r="ABI36" s="0"/>
-      <c r="ABJ36" s="0"/>
-      <c r="ABK36" s="0"/>
-      <c r="ABL36" s="0"/>
-      <c r="ABM36" s="0"/>
-      <c r="ABN36" s="0"/>
-      <c r="ABO36" s="0"/>
-      <c r="ABP36" s="0"/>
-      <c r="ABQ36" s="0"/>
-      <c r="ABR36" s="0"/>
-      <c r="ABS36" s="0"/>
-      <c r="ABT36" s="0"/>
-      <c r="ABU36" s="0"/>
-      <c r="ABV36" s="0"/>
-      <c r="ABW36" s="0"/>
-      <c r="ABX36" s="0"/>
-      <c r="ABY36" s="0"/>
-      <c r="ABZ36" s="0"/>
-      <c r="ACA36" s="0"/>
-      <c r="ACB36" s="0"/>
-      <c r="ACC36" s="0"/>
-      <c r="ACD36" s="0"/>
-      <c r="ACE36" s="0"/>
-      <c r="ACF36" s="0"/>
-      <c r="ACG36" s="0"/>
-      <c r="ACH36" s="0"/>
-      <c r="ACI36" s="0"/>
-      <c r="ACJ36" s="0"/>
-      <c r="ACK36" s="0"/>
-      <c r="ACL36" s="0"/>
-      <c r="ACM36" s="0"/>
-      <c r="ACN36" s="0"/>
-      <c r="ACO36" s="0"/>
-      <c r="ACP36" s="0"/>
-      <c r="ACQ36" s="0"/>
-      <c r="ACR36" s="0"/>
-      <c r="ACS36" s="0"/>
-      <c r="ACT36" s="0"/>
-      <c r="ACU36" s="0"/>
-      <c r="ACV36" s="0"/>
-      <c r="ACW36" s="0"/>
-      <c r="ACX36" s="0"/>
-      <c r="ACY36" s="0"/>
-      <c r="ACZ36" s="0"/>
-      <c r="ADA36" s="0"/>
-      <c r="ADB36" s="0"/>
-      <c r="ADC36" s="0"/>
-      <c r="ADD36" s="0"/>
-      <c r="ADE36" s="0"/>
-      <c r="ADF36" s="0"/>
-      <c r="ADG36" s="0"/>
-      <c r="ADH36" s="0"/>
-      <c r="ADI36" s="0"/>
-      <c r="ADJ36" s="0"/>
-      <c r="ADK36" s="0"/>
-      <c r="ADL36" s="0"/>
-      <c r="ADM36" s="0"/>
-      <c r="ADN36" s="0"/>
-      <c r="ADO36" s="0"/>
-      <c r="ADP36" s="0"/>
-      <c r="ADQ36" s="0"/>
-      <c r="ADR36" s="0"/>
-      <c r="ADS36" s="0"/>
-      <c r="ADT36" s="0"/>
-      <c r="ADU36" s="0"/>
-      <c r="ADV36" s="0"/>
-      <c r="ADW36" s="0"/>
-      <c r="ADX36" s="0"/>
-      <c r="ADY36" s="0"/>
-      <c r="ADZ36" s="0"/>
-      <c r="AEA36" s="0"/>
-      <c r="AEB36" s="0"/>
-      <c r="AEC36" s="0"/>
-      <c r="AED36" s="0"/>
-      <c r="AEE36" s="0"/>
-      <c r="AEF36" s="0"/>
-      <c r="AEG36" s="0"/>
-      <c r="AEH36" s="0"/>
-      <c r="AEI36" s="0"/>
-      <c r="AEJ36" s="0"/>
-      <c r="AEK36" s="0"/>
-      <c r="AEL36" s="0"/>
-      <c r="AEM36" s="0"/>
-      <c r="AEN36" s="0"/>
-      <c r="AEO36" s="0"/>
-      <c r="AEP36" s="0"/>
-      <c r="AEQ36" s="0"/>
-      <c r="AER36" s="0"/>
-      <c r="AES36" s="0"/>
-      <c r="AET36" s="0"/>
-      <c r="AEU36" s="0"/>
-      <c r="AEV36" s="0"/>
-      <c r="AEW36" s="0"/>
-      <c r="AEX36" s="0"/>
-      <c r="AEY36" s="0"/>
-      <c r="AEZ36" s="0"/>
-      <c r="AFA36" s="0"/>
-      <c r="AFB36" s="0"/>
-      <c r="AFC36" s="0"/>
-      <c r="AFD36" s="0"/>
-      <c r="AFE36" s="0"/>
-      <c r="AFF36" s="0"/>
-      <c r="AFG36" s="0"/>
-      <c r="AFH36" s="0"/>
-      <c r="AFI36" s="0"/>
-      <c r="AFJ36" s="0"/>
-      <c r="AFK36" s="0"/>
-      <c r="AFL36" s="0"/>
-      <c r="AFM36" s="0"/>
-      <c r="AFN36" s="0"/>
-      <c r="AFO36" s="0"/>
-      <c r="AFP36" s="0"/>
-      <c r="AFQ36" s="0"/>
-      <c r="AFR36" s="0"/>
-      <c r="AFS36" s="0"/>
-      <c r="AFT36" s="0"/>
-      <c r="AFU36" s="0"/>
-      <c r="AFV36" s="0"/>
-      <c r="AFW36" s="0"/>
-      <c r="AFX36" s="0"/>
-      <c r="AFY36" s="0"/>
-      <c r="AFZ36" s="0"/>
-      <c r="AGA36" s="0"/>
-      <c r="AGB36" s="0"/>
-      <c r="AGC36" s="0"/>
-      <c r="AGD36" s="0"/>
-      <c r="AGE36" s="0"/>
-      <c r="AGF36" s="0"/>
-      <c r="AGG36" s="0"/>
-      <c r="AGH36" s="0"/>
-      <c r="AGI36" s="0"/>
-      <c r="AGJ36" s="0"/>
-      <c r="AGK36" s="0"/>
-      <c r="AGL36" s="0"/>
-      <c r="AGM36" s="0"/>
-      <c r="AGN36" s="0"/>
-      <c r="AGO36" s="0"/>
-      <c r="AGP36" s="0"/>
-      <c r="AGQ36" s="0"/>
-      <c r="AGR36" s="0"/>
-      <c r="AGS36" s="0"/>
-      <c r="AGT36" s="0"/>
-      <c r="AGU36" s="0"/>
-      <c r="AGV36" s="0"/>
-      <c r="AGW36" s="0"/>
-      <c r="AGX36" s="0"/>
-      <c r="AGY36" s="0"/>
-      <c r="AGZ36" s="0"/>
-      <c r="AHA36" s="0"/>
-      <c r="AHB36" s="0"/>
-      <c r="AHC36" s="0"/>
-      <c r="AHD36" s="0"/>
-      <c r="AHE36" s="0"/>
-      <c r="AHF36" s="0"/>
-      <c r="AHG36" s="0"/>
-      <c r="AHH36" s="0"/>
-      <c r="AHI36" s="0"/>
-      <c r="AHJ36" s="0"/>
-      <c r="AHK36" s="0"/>
-      <c r="AHL36" s="0"/>
-      <c r="AHM36" s="0"/>
-      <c r="AHN36" s="0"/>
-      <c r="AHO36" s="0"/>
-      <c r="AHP36" s="0"/>
-      <c r="AHQ36" s="0"/>
-      <c r="AHR36" s="0"/>
-      <c r="AHS36" s="0"/>
-      <c r="AHT36" s="0"/>
-      <c r="AHU36" s="0"/>
-      <c r="AHV36" s="0"/>
-      <c r="AHW36" s="0"/>
-      <c r="AHX36" s="0"/>
-      <c r="AHY36" s="0"/>
-      <c r="AHZ36" s="0"/>
-      <c r="AIA36" s="0"/>
-      <c r="AIB36" s="0"/>
-      <c r="AIC36" s="0"/>
-      <c r="AID36" s="0"/>
-      <c r="AIE36" s="0"/>
-      <c r="AIF36" s="0"/>
-      <c r="AIG36" s="0"/>
-      <c r="AIH36" s="0"/>
-      <c r="AII36" s="0"/>
-      <c r="AIJ36" s="0"/>
-      <c r="AIK36" s="0"/>
-      <c r="AIL36" s="0"/>
-      <c r="AIM36" s="0"/>
-      <c r="AIN36" s="0"/>
-      <c r="AIO36" s="0"/>
-      <c r="AIP36" s="0"/>
-      <c r="AIQ36" s="0"/>
-      <c r="AIR36" s="0"/>
-      <c r="AIS36" s="0"/>
-      <c r="AIT36" s="0"/>
-      <c r="AIU36" s="0"/>
-      <c r="AIV36" s="0"/>
-      <c r="AIW36" s="0"/>
-      <c r="AIX36" s="0"/>
-      <c r="AIY36" s="0"/>
-      <c r="AIZ36" s="0"/>
-      <c r="AJA36" s="0"/>
-      <c r="AJB36" s="0"/>
-      <c r="AJC36" s="0"/>
-      <c r="AJD36" s="0"/>
-      <c r="AJE36" s="0"/>
-      <c r="AJF36" s="0"/>
-      <c r="AJG36" s="0"/>
-      <c r="AJH36" s="0"/>
-      <c r="AJI36" s="0"/>
-      <c r="AJJ36" s="0"/>
-      <c r="AJK36" s="0"/>
-      <c r="AJL36" s="0"/>
-      <c r="AJM36" s="0"/>
-      <c r="AJN36" s="0"/>
-      <c r="AJO36" s="0"/>
-      <c r="AJP36" s="0"/>
-      <c r="AJQ36" s="0"/>
-      <c r="AJR36" s="0"/>
-      <c r="AJS36" s="0"/>
-      <c r="AJT36" s="0"/>
-      <c r="AJU36" s="0"/>
-      <c r="AJV36" s="0"/>
-      <c r="AJW36" s="0"/>
-      <c r="AJX36" s="0"/>
-      <c r="AJY36" s="0"/>
-      <c r="AJZ36" s="0"/>
-      <c r="AKA36" s="0"/>
-      <c r="AKB36" s="0"/>
-      <c r="AKC36" s="0"/>
-      <c r="AKD36" s="0"/>
-      <c r="AKE36" s="0"/>
-      <c r="AKF36" s="0"/>
-      <c r="AKG36" s="0"/>
-      <c r="AKH36" s="0"/>
-      <c r="AKI36" s="0"/>
-      <c r="AKJ36" s="0"/>
-      <c r="AKK36" s="0"/>
-      <c r="AKL36" s="0"/>
-      <c r="AKM36" s="0"/>
-      <c r="AKN36" s="0"/>
-      <c r="AKO36" s="0"/>
-      <c r="AKP36" s="0"/>
-      <c r="AKQ36" s="0"/>
-      <c r="AKR36" s="0"/>
-      <c r="AKS36" s="0"/>
-      <c r="AKT36" s="0"/>
-      <c r="AKU36" s="0"/>
-      <c r="AKV36" s="0"/>
-      <c r="AKW36" s="0"/>
-      <c r="AKX36" s="0"/>
-      <c r="AKY36" s="0"/>
-      <c r="AKZ36" s="0"/>
-      <c r="ALA36" s="0"/>
-      <c r="ALB36" s="0"/>
-      <c r="ALC36" s="0"/>
-      <c r="ALD36" s="0"/>
-      <c r="ALE36" s="0"/>
-      <c r="ALF36" s="0"/>
-      <c r="ALG36" s="0"/>
-      <c r="ALH36" s="0"/>
-      <c r="ALI36" s="0"/>
-      <c r="ALJ36" s="0"/>
-      <c r="ALK36" s="0"/>
-      <c r="ALL36" s="0"/>
-      <c r="ALM36" s="0"/>
-      <c r="ALN36" s="0"/>
-      <c r="ALO36" s="0"/>
-      <c r="ALP36" s="0"/>
-      <c r="ALQ36" s="0"/>
-      <c r="ALR36" s="0"/>
-      <c r="ALS36" s="0"/>
-      <c r="ALT36" s="0"/>
-      <c r="ALU36" s="0"/>
-      <c r="ALV36" s="0"/>
-      <c r="ALW36" s="0"/>
-      <c r="ALX36" s="0"/>
-      <c r="ALY36" s="0"/>
-      <c r="ALZ36" s="0"/>
-      <c r="AMA36" s="0"/>
-      <c r="AMB36" s="0"/>
-      <c r="AMC36" s="0"/>
-      <c r="AMD36" s="0"/>
-      <c r="AME36" s="0"/>
-      <c r="AMF36" s="0"/>
-      <c r="AMG36" s="0"/>
-      <c r="AMH36" s="0"/>
-      <c r="AMI36" s="0"/>
-      <c r="AMJ36" s="0"/>
-    </row>
-    <row r="37" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12" t="s">
+      <c r="C36" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="21" t="s">
+      <c r="D36" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="26" t="s">
+      <c r="E36" s="21"/>
+      <c r="F36" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="G36" s="0"/>
+      <c r="H36" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="26" t="s">
+      <c r="I36" s="21"/>
+      <c r="J36" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="0"/>
-      <c r="H38" s="26" t="s">
+      <c r="K36" s="0"/>
+      <c r="L36" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="21"/>
-      <c r="J38" s="26" t="s">
+      <c r="M36" s="21"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="K38" s="0"/>
-      <c r="L38" s="26" t="s">
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="M38" s="21"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21" t="s">
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="0"/>
+      <c r="K37" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="26" t="s">
+      <c r="L37" s="21"/>
+      <c r="M37" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="0"/>
-      <c r="K39" s="26" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="L39" s="21"/>
-      <c r="M39" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="22"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
-      <c r="M40" s="22"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.2" right="0.2" top="0.170138888888889" bottom="0.159722222222222" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>